<commit_message>
update to UART et rangement
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xilinx_project\CPUproject\projet_CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xilinx_project\git_project\projet_CPU\projet_CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069C36AB-63CB-403E-9230-D027C63E20AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45C6131-12CB-471A-845C-078D53AF4A75}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="4545" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="1320" windowWidth="24075" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Format operateur" sheetId="1" r:id="rId1"/>
     <sheet name="PLL_PWM compute" sheetId="4" r:id="rId2"/>
     <sheet name="Cache" sheetId="5" r:id="rId3"/>
-    <sheet name="cache(2)" sheetId="6" r:id="rId4"/>
-    <sheet name="Fomat registre" sheetId="2" r:id="rId5"/>
-    <sheet name="Operateur" sheetId="3" r:id="rId6"/>
+    <sheet name="Feuil1" sheetId="7" r:id="rId4"/>
+    <sheet name="cache(2)" sheetId="6" r:id="rId5"/>
+    <sheet name="Fomat registre" sheetId="2" r:id="rId6"/>
+    <sheet name="Operateur" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="291">
   <si>
     <t>ADD</t>
   </si>
@@ -902,6 +903,12 @@
   </si>
   <si>
     <t>addr_down_lvl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HandShake </t>
+  </si>
+  <si>
+    <t>(ACK est controllé par le master/(le 1 reset tout le monde)</t>
   </si>
 </sst>
 </file>
@@ -1005,10 +1012,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2419,26 +2426,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="R9:Y9"/>
-    <mergeCell ref="Z9:AG9"/>
-    <mergeCell ref="B9:Q9"/>
-    <mergeCell ref="B10:Q10"/>
-    <mergeCell ref="R10:Y10"/>
-    <mergeCell ref="Z10:AG10"/>
-    <mergeCell ref="Z11:AG11"/>
-    <mergeCell ref="J11:Y11"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="J12:Q12"/>
-    <mergeCell ref="R12:AG12"/>
-    <mergeCell ref="Z8:AG8"/>
-    <mergeCell ref="Z7:AG7"/>
-    <mergeCell ref="R7:Y7"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="J8:Q8"/>
-    <mergeCell ref="R8:Y8"/>
     <mergeCell ref="I6:AG6"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="B6:D6"/>
@@ -2455,6 +2442,26 @@
     <mergeCell ref="X2:AB2"/>
     <mergeCell ref="S2:W2"/>
     <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="Z8:AG8"/>
+    <mergeCell ref="Z7:AG7"/>
+    <mergeCell ref="R7:Y7"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="J8:Q8"/>
+    <mergeCell ref="R8:Y8"/>
+    <mergeCell ref="Z11:AG11"/>
+    <mergeCell ref="J11:Y11"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="J12:Q12"/>
+    <mergeCell ref="R12:AG12"/>
+    <mergeCell ref="R9:Y9"/>
+    <mergeCell ref="Z9:AG9"/>
+    <mergeCell ref="B9:Q9"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="R10:Y10"/>
+    <mergeCell ref="Z10:AG10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2639,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C217D931-D8EC-4E18-86A1-839AA8BD0689}">
   <dimension ref="A3:U39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3134,10 +3141,291 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC584C10-E2F9-497C-8849-09E92E2CAC95}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" t="s">
+        <v>289</v>
+      </c>
+      <c r="E11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C6F1E8-74C4-4BB6-8AC3-414BA2E5596B}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -3240,7 +3528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
@@ -3507,7 +3795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BA109"/>
   <sheetViews>
@@ -3743,20 +4031,20 @@
       <c r="S3" s="4">
         <v>0</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="16" t="s">
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z3" s="16"/>
-      <c r="AA3" s="16"/>
-      <c r="AB3" s="16"/>
-      <c r="AC3" s="16"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+      <c r="AC3" s="15"/>
       <c r="AD3" s="14" t="s">
         <v>1</v>
       </c>
@@ -3823,20 +4111,20 @@
       <c r="S4" s="4">
         <v>1</v>
       </c>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="16" t="s">
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15"/>
       <c r="AD4" s="14" t="s">
         <v>1</v>
       </c>
@@ -3927,20 +4215,20 @@
       <c r="S5" s="4">
         <v>0</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="16" t="s">
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
       <c r="AD5" s="14" t="s">
         <v>1</v>
       </c>
@@ -4016,20 +4304,20 @@
       <c r="S6" s="4">
         <v>1</v>
       </c>
-      <c r="T6" s="15" t="s">
+      <c r="T6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="16" t="s">
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
       <c r="AD6" s="14" t="s">
         <v>1</v>
       </c>
@@ -4105,20 +4393,20 @@
       <c r="S7" s="4">
         <v>0</v>
       </c>
-      <c r="T7" s="15" t="s">
+      <c r="T7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="16" t="s">
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
       <c r="AD7" s="14" t="s">
         <v>1</v>
       </c>
@@ -4197,20 +4485,20 @@
       <c r="S8" s="4">
         <v>1</v>
       </c>
-      <c r="T8" s="15" t="s">
+      <c r="T8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="16" t="s">
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
       <c r="AD8" s="14" t="s">
         <v>1</v>
       </c>
@@ -4286,20 +4574,20 @@
       <c r="S9" s="4">
         <v>0</v>
       </c>
-      <c r="T9" s="15" t="s">
+      <c r="T9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="16" t="s">
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
       <c r="AD9" s="14" t="s">
         <v>1</v>
       </c>
@@ -4375,20 +4663,20 @@
       <c r="S10" s="4">
         <v>1</v>
       </c>
-      <c r="T10" s="15" t="s">
+      <c r="T10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="16" t="s">
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-      <c r="AC10" s="16"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
       <c r="AD10" s="14" t="s">
         <v>1</v>
       </c>
@@ -4464,20 +4752,20 @@
       <c r="S11" s="4">
         <v>0</v>
       </c>
-      <c r="T11" s="15" t="s">
+      <c r="T11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="16" t="s">
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z11" s="16"/>
-      <c r="AA11" s="16"/>
-      <c r="AB11" s="16"/>
-      <c r="AC11" s="16"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
       <c r="AD11" s="14" t="s">
         <v>1</v>
       </c>
@@ -4553,20 +4841,20 @@
       <c r="S12" s="4">
         <v>1</v>
       </c>
-      <c r="T12" s="15" t="s">
+      <c r="T12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="16" t="s">
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z12" s="16"/>
-      <c r="AA12" s="16"/>
-      <c r="AB12" s="16"/>
-      <c r="AC12" s="16"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
       <c r="AD12" s="14" t="s">
         <v>1</v>
       </c>
@@ -4642,20 +4930,20 @@
       <c r="S13" s="4">
         <v>0</v>
       </c>
-      <c r="T13" s="15" t="s">
+      <c r="T13" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="16" t="s">
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z13" s="16"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="16"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
       <c r="AD13" s="14" t="s">
         <v>1</v>
       </c>
@@ -4731,20 +5019,20 @@
       <c r="S14" s="4">
         <v>1</v>
       </c>
-      <c r="T14" s="15" t="s">
+      <c r="T14" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="16" t="s">
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="16"/>
-      <c r="AC14" s="16"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
       <c r="AD14" s="14" t="s">
         <v>1</v>
       </c>
@@ -4820,20 +5108,20 @@
       <c r="S15" s="4">
         <v>0</v>
       </c>
-      <c r="T15" s="15" t="s">
+      <c r="T15" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="16" t="s">
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z15" s="16"/>
-      <c r="AA15" s="16"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="16"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
       <c r="AD15" s="14" t="s">
         <v>1</v>
       </c>
@@ -4909,20 +5197,20 @@
       <c r="S16" s="4">
         <v>1</v>
       </c>
-      <c r="T16" s="15" t="s">
+      <c r="T16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="16" t="s">
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z16" s="16"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="16"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
       <c r="AD16" s="14" t="s">
         <v>1</v>
       </c>
@@ -4998,20 +5286,20 @@
       <c r="S17" s="4">
         <v>0</v>
       </c>
-      <c r="T17" s="15" t="s">
+      <c r="T17" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="16" t="s">
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="16"/>
-      <c r="AC17" s="16"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
       <c r="AD17" s="14" t="s">
         <v>1</v>
       </c>
@@ -5087,20 +5375,20 @@
       <c r="S18" s="4">
         <v>1</v>
       </c>
-      <c r="T18" s="15" t="s">
+      <c r="T18" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="16" t="s">
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="W18" s="16"/>
+      <c r="X18" s="16"/>
+      <c r="Y18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
       <c r="AD18" s="14" t="s">
         <v>1</v>
       </c>
@@ -5176,20 +5464,20 @@
       <c r="S19" s="4">
         <v>0</v>
       </c>
-      <c r="T19" s="15" t="s">
+      <c r="T19" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="16" t="s">
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
+      <c r="W19" s="16"/>
+      <c r="X19" s="16"/>
+      <c r="Y19" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z19" s="16"/>
-      <c r="AA19" s="16"/>
-      <c r="AB19" s="16"/>
-      <c r="AC19" s="16"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
       <c r="AD19" s="14" t="s">
         <v>1</v>
       </c>
@@ -5265,20 +5553,20 @@
       <c r="S20" s="4">
         <v>1</v>
       </c>
-      <c r="T20" s="15" t="s">
+      <c r="T20" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="16" t="s">
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z20" s="16"/>
-      <c r="AA20" s="16"/>
-      <c r="AB20" s="16"/>
-      <c r="AC20" s="16"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
       <c r="AD20" s="14" t="s">
         <v>1</v>
       </c>
@@ -5354,20 +5642,20 @@
       <c r="S21" s="4">
         <v>0</v>
       </c>
-      <c r="T21" s="15" t="s">
+      <c r="T21" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="16" t="s">
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z21" s="16"/>
-      <c r="AA21" s="16"/>
-      <c r="AB21" s="16"/>
-      <c r="AC21" s="16"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="15"/>
       <c r="AD21" s="14" t="s">
         <v>1</v>
       </c>
@@ -5443,20 +5731,20 @@
       <c r="S22" s="4">
         <v>1</v>
       </c>
-      <c r="T22" s="15" t="s">
+      <c r="T22" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="16" t="s">
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z22" s="16"/>
-      <c r="AA22" s="16"/>
-      <c r="AB22" s="16"/>
-      <c r="AC22" s="16"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
       <c r="AD22" s="14" t="s">
         <v>1</v>
       </c>
@@ -5532,20 +5820,20 @@
       <c r="S23" s="4">
         <v>0</v>
       </c>
-      <c r="T23" s="15" t="s">
+      <c r="T23" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="16" t="s">
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z23" s="16"/>
-      <c r="AA23" s="16"/>
-      <c r="AB23" s="16"/>
-      <c r="AC23" s="16"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
       <c r="AD23" s="14" t="s">
         <v>1</v>
       </c>
@@ -5624,20 +5912,20 @@
       <c r="S24" s="4">
         <v>1</v>
       </c>
-      <c r="T24" s="15" t="s">
+      <c r="T24" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="16" t="s">
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z24" s="16"/>
-      <c r="AA24" s="16"/>
-      <c r="AB24" s="16"/>
-      <c r="AC24" s="16"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
       <c r="AD24" s="14" t="s">
         <v>1</v>
       </c>
@@ -5713,20 +6001,20 @@
       <c r="S25" s="4">
         <v>0</v>
       </c>
-      <c r="T25" s="15" t="s">
+      <c r="T25" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="16" t="s">
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z25" s="16"/>
-      <c r="AA25" s="16"/>
-      <c r="AB25" s="16"/>
-      <c r="AC25" s="16"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="15"/>
+      <c r="AC25" s="15"/>
       <c r="AD25" s="14" t="s">
         <v>1</v>
       </c>
@@ -5802,20 +6090,20 @@
       <c r="S26" s="4">
         <v>1</v>
       </c>
-      <c r="T26" s="15" t="s">
+      <c r="T26" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U26" s="15"/>
-      <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="15"/>
-      <c r="Y26" s="16" t="s">
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z26" s="16"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="16"/>
-      <c r="AC26" s="16"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="15"/>
       <c r="AD26" s="14" t="s">
         <v>1</v>
       </c>
@@ -5888,20 +6176,20 @@
       <c r="S27" s="4">
         <v>0</v>
       </c>
-      <c r="T27" s="15" t="s">
+      <c r="T27" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="16" t="s">
+      <c r="U27" s="16"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+      <c r="Y27" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z27" s="16"/>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="16"/>
-      <c r="AC27" s="16"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="15"/>
+      <c r="AB27" s="15"/>
+      <c r="AC27" s="15"/>
       <c r="AD27" s="14" t="s">
         <v>1</v>
       </c>
@@ -5977,20 +6265,20 @@
       <c r="S28" s="4">
         <v>1</v>
       </c>
-      <c r="T28" s="15" t="s">
+      <c r="T28" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="16" t="s">
+      <c r="U28" s="16"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="16"/>
+      <c r="Y28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z28" s="16"/>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="16"/>
-      <c r="AC28" s="16"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
       <c r="AD28" s="14" t="s">
         <v>1</v>
       </c>
@@ -6066,20 +6354,20 @@
       <c r="S29" s="4">
         <v>0</v>
       </c>
-      <c r="T29" s="15" t="s">
+      <c r="T29" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="16" t="s">
+      <c r="U29" s="16"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16"/>
+      <c r="X29" s="16"/>
+      <c r="Y29" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z29" s="16"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="16"/>
-      <c r="AC29" s="16"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="15"/>
+      <c r="AB29" s="15"/>
+      <c r="AC29" s="15"/>
       <c r="AD29" s="14" t="s">
         <v>1</v>
       </c>
@@ -6155,20 +6443,20 @@
       <c r="S30" s="4">
         <v>1</v>
       </c>
-      <c r="T30" s="15" t="s">
+      <c r="T30" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="16" t="s">
+      <c r="U30" s="16"/>
+      <c r="V30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="16"/>
+      <c r="Y30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z30" s="16"/>
-      <c r="AA30" s="16"/>
-      <c r="AB30" s="16"/>
-      <c r="AC30" s="16"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="15"/>
       <c r="AD30" s="14" t="s">
         <v>1</v>
       </c>
@@ -6244,20 +6532,20 @@
       <c r="S31" s="4">
         <v>0</v>
       </c>
-      <c r="T31" s="15" t="s">
+      <c r="T31" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="16" t="s">
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
+      <c r="X31" s="16"/>
+      <c r="Y31" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z31" s="16"/>
-      <c r="AA31" s="16"/>
-      <c r="AB31" s="16"/>
-      <c r="AC31" s="16"/>
+      <c r="Z31" s="15"/>
+      <c r="AA31" s="15"/>
+      <c r="AB31" s="15"/>
+      <c r="AC31" s="15"/>
       <c r="AD31" s="14" t="s">
         <v>1</v>
       </c>
@@ -6333,20 +6621,20 @@
       <c r="S32" s="4">
         <v>1</v>
       </c>
-      <c r="T32" s="15" t="s">
+      <c r="T32" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="16" t="s">
+      <c r="U32" s="16"/>
+      <c r="V32" s="16"/>
+      <c r="W32" s="16"/>
+      <c r="X32" s="16"/>
+      <c r="Y32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z32" s="16"/>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="16"/>
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="15"/>
+      <c r="AB32" s="15"/>
+      <c r="AC32" s="15"/>
       <c r="AD32" s="14" t="s">
         <v>1</v>
       </c>
@@ -6422,20 +6710,20 @@
       <c r="S33" s="4">
         <v>0</v>
       </c>
-      <c r="T33" s="15" t="s">
+      <c r="T33" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U33" s="15"/>
-      <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
-      <c r="X33" s="15"/>
-      <c r="Y33" s="16" t="s">
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z33" s="16"/>
-      <c r="AA33" s="16"/>
-      <c r="AB33" s="16"/>
-      <c r="AC33" s="16"/>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
+      <c r="AC33" s="15"/>
       <c r="AD33" s="14" t="s">
         <v>1</v>
       </c>
@@ -6511,20 +6799,20 @@
       <c r="S34" s="4">
         <v>1</v>
       </c>
-      <c r="T34" s="15" t="s">
+      <c r="T34" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U34" s="15"/>
-      <c r="V34" s="15"/>
-      <c r="W34" s="15"/>
-      <c r="X34" s="15"/>
-      <c r="Y34" s="16" t="s">
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="16"/>
+      <c r="Y34" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Z34" s="16"/>
-      <c r="AA34" s="16"/>
-      <c r="AB34" s="16"/>
-      <c r="AC34" s="16"/>
+      <c r="Z34" s="15"/>
+      <c r="AA34" s="15"/>
+      <c r="AB34" s="15"/>
+      <c r="AC34" s="15"/>
       <c r="AD34" s="14" t="s">
         <v>1</v>
       </c>
@@ -6597,20 +6885,20 @@
       <c r="S35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="T35" s="15" t="s">
+      <c r="T35" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="16" t="s">
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="Z35" s="16"/>
-      <c r="AA35" s="16"/>
-      <c r="AB35" s="16"/>
-      <c r="AC35" s="16"/>
+      <c r="Z35" s="15"/>
+      <c r="AA35" s="15"/>
+      <c r="AB35" s="15"/>
+      <c r="AC35" s="15"/>
       <c r="AD35" s="14" t="s">
         <v>1</v>
       </c>
@@ -6686,20 +6974,20 @@
       <c r="S36" s="4">
         <v>0</v>
       </c>
-      <c r="T36" s="15" t="s">
+      <c r="T36" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="16" t="s">
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z36" s="16"/>
-      <c r="AA36" s="16"/>
-      <c r="AB36" s="16"/>
-      <c r="AC36" s="16"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
       <c r="AD36" s="14" t="s">
         <v>1</v>
       </c>
@@ -6775,20 +7063,20 @@
       <c r="S37" s="4">
         <v>1</v>
       </c>
-      <c r="T37" s="15" t="s">
+      <c r="T37" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U37" s="15"/>
-      <c r="V37" s="15"/>
-      <c r="W37" s="15"/>
-      <c r="X37" s="15"/>
-      <c r="Y37" s="16" t="s">
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="16"/>
+      <c r="Y37" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z37" s="16"/>
-      <c r="AA37" s="16"/>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="16"/>
+      <c r="Z37" s="15"/>
+      <c r="AA37" s="15"/>
+      <c r="AB37" s="15"/>
+      <c r="AC37" s="15"/>
       <c r="AD37" s="14" t="s">
         <v>1</v>
       </c>
@@ -6864,20 +7152,20 @@
       <c r="S38" s="4">
         <v>0</v>
       </c>
-      <c r="T38" s="15" t="s">
+      <c r="T38" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="16" t="s">
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
+      <c r="Y38" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z38" s="16"/>
-      <c r="AA38" s="16"/>
-      <c r="AB38" s="16"/>
-      <c r="AC38" s="16"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
       <c r="AD38" s="14" t="s">
         <v>1</v>
       </c>
@@ -6953,20 +7241,20 @@
       <c r="S39" s="4">
         <v>1</v>
       </c>
-      <c r="T39" s="15" t="s">
+      <c r="T39" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U39" s="15"/>
-      <c r="V39" s="15"/>
-      <c r="W39" s="15"/>
-      <c r="X39" s="15"/>
-      <c r="Y39" s="16" t="s">
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z39" s="16"/>
-      <c r="AA39" s="16"/>
-      <c r="AB39" s="16"/>
-      <c r="AC39" s="16"/>
+      <c r="Z39" s="15"/>
+      <c r="AA39" s="15"/>
+      <c r="AB39" s="15"/>
+      <c r="AC39" s="15"/>
       <c r="AD39" s="14" t="s">
         <v>1</v>
       </c>
@@ -7042,20 +7330,20 @@
       <c r="S40" s="4">
         <v>0</v>
       </c>
-      <c r="T40" s="15" t="s">
+      <c r="T40" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="15"/>
-      <c r="Y40" s="16" t="s">
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="16"/>
+      <c r="Y40" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z40" s="16"/>
-      <c r="AA40" s="16"/>
-      <c r="AB40" s="16"/>
-      <c r="AC40" s="16"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
       <c r="AD40" s="14" t="s">
         <v>1</v>
       </c>
@@ -7131,20 +7419,20 @@
       <c r="S41" s="4">
         <v>1</v>
       </c>
-      <c r="T41" s="15" t="s">
+      <c r="T41" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="15"/>
-      <c r="X41" s="15"/>
-      <c r="Y41" s="16" t="s">
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="16"/>
+      <c r="Y41" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z41" s="16"/>
-      <c r="AA41" s="16"/>
-      <c r="AB41" s="16"/>
-      <c r="AC41" s="16"/>
+      <c r="Z41" s="15"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="15"/>
       <c r="AD41" s="14" t="s">
         <v>75</v>
       </c>
@@ -7220,20 +7508,20 @@
       <c r="S42" s="4">
         <v>0</v>
       </c>
-      <c r="T42" s="15" t="s">
+      <c r="T42" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U42" s="15"/>
-      <c r="V42" s="15"/>
-      <c r="W42" s="15"/>
-      <c r="X42" s="15"/>
-      <c r="Y42" s="16" t="s">
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="16"/>
+      <c r="X42" s="16"/>
+      <c r="Y42" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z42" s="16"/>
-      <c r="AA42" s="16"/>
-      <c r="AB42" s="16"/>
-      <c r="AC42" s="16"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
       <c r="AD42" s="14" t="s">
         <v>75</v>
       </c>
@@ -7309,20 +7597,20 @@
       <c r="S43" s="4">
         <v>1</v>
       </c>
-      <c r="T43" s="15" t="s">
+      <c r="T43" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="16" t="s">
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z43" s="16"/>
-      <c r="AA43" s="16"/>
-      <c r="AB43" s="16"/>
-      <c r="AC43" s="16"/>
+      <c r="Z43" s="15"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
       <c r="AD43" s="14" t="s">
         <v>1</v>
       </c>
@@ -7398,20 +7686,20 @@
       <c r="S44" s="4">
         <v>0</v>
       </c>
-      <c r="T44" s="15" t="s">
+      <c r="T44" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="16" t="s">
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
+      <c r="W44" s="16"/>
+      <c r="X44" s="16"/>
+      <c r="Y44" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z44" s="16"/>
-      <c r="AA44" s="16"/>
-      <c r="AB44" s="16"/>
-      <c r="AC44" s="16"/>
+      <c r="Z44" s="15"/>
+      <c r="AA44" s="15"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
       <c r="AD44" s="14" t="s">
         <v>1</v>
       </c>
@@ -7487,20 +7775,20 @@
       <c r="S45" s="4">
         <v>1</v>
       </c>
-      <c r="T45" s="15" t="s">
+      <c r="T45" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U45" s="15"/>
-      <c r="V45" s="15"/>
-      <c r="W45" s="15"/>
-      <c r="X45" s="15"/>
-      <c r="Y45" s="16" t="s">
+      <c r="U45" s="16"/>
+      <c r="V45" s="16"/>
+      <c r="W45" s="16"/>
+      <c r="X45" s="16"/>
+      <c r="Y45" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z45" s="16"/>
-      <c r="AA45" s="16"/>
-      <c r="AB45" s="16"/>
-      <c r="AC45" s="16"/>
+      <c r="Z45" s="15"/>
+      <c r="AA45" s="15"/>
+      <c r="AB45" s="15"/>
+      <c r="AC45" s="15"/>
       <c r="AD45" s="14" t="s">
         <v>75</v>
       </c>
@@ -7576,20 +7864,20 @@
       <c r="S46" s="4">
         <v>0</v>
       </c>
-      <c r="T46" s="15" t="s">
+      <c r="T46" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U46" s="15"/>
-      <c r="V46" s="15"/>
-      <c r="W46" s="15"/>
-      <c r="X46" s="15"/>
-      <c r="Y46" s="16" t="s">
+      <c r="U46" s="16"/>
+      <c r="V46" s="16"/>
+      <c r="W46" s="16"/>
+      <c r="X46" s="16"/>
+      <c r="Y46" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z46" s="16"/>
-      <c r="AA46" s="16"/>
-      <c r="AB46" s="16"/>
-      <c r="AC46" s="16"/>
+      <c r="Z46" s="15"/>
+      <c r="AA46" s="15"/>
+      <c r="AB46" s="15"/>
+      <c r="AC46" s="15"/>
       <c r="AD46" s="14" t="s">
         <v>1</v>
       </c>
@@ -7665,20 +7953,20 @@
       <c r="S47" s="4">
         <v>1</v>
       </c>
-      <c r="T47" s="15" t="s">
+      <c r="T47" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U47" s="15"/>
-      <c r="V47" s="15"/>
-      <c r="W47" s="15"/>
-      <c r="X47" s="15"/>
-      <c r="Y47" s="16" t="s">
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
+      <c r="W47" s="16"/>
+      <c r="X47" s="16"/>
+      <c r="Y47" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z47" s="16"/>
-      <c r="AA47" s="16"/>
-      <c r="AB47" s="16"/>
-      <c r="AC47" s="16"/>
+      <c r="Z47" s="15"/>
+      <c r="AA47" s="15"/>
+      <c r="AB47" s="15"/>
+      <c r="AC47" s="15"/>
       <c r="AD47" s="14" t="s">
         <v>1</v>
       </c>
@@ -7754,20 +8042,20 @@
       <c r="S48" s="4">
         <v>0</v>
       </c>
-      <c r="T48" s="15" t="s">
+      <c r="T48" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U48" s="15"/>
-      <c r="V48" s="15"/>
-      <c r="W48" s="15"/>
-      <c r="X48" s="15"/>
-      <c r="Y48" s="16" t="s">
+      <c r="U48" s="16"/>
+      <c r="V48" s="16"/>
+      <c r="W48" s="16"/>
+      <c r="X48" s="16"/>
+      <c r="Y48" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z48" s="16"/>
-      <c r="AA48" s="16"/>
-      <c r="AB48" s="16"/>
-      <c r="AC48" s="16"/>
+      <c r="Z48" s="15"/>
+      <c r="AA48" s="15"/>
+      <c r="AB48" s="15"/>
+      <c r="AC48" s="15"/>
       <c r="AD48" s="14" t="s">
         <v>1</v>
       </c>
@@ -7844,20 +8132,20 @@
       <c r="S49" s="4">
         <v>1</v>
       </c>
-      <c r="T49" s="15" t="s">
+      <c r="T49" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U49" s="15"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="16" t="s">
+      <c r="U49" s="16"/>
+      <c r="V49" s="16"/>
+      <c r="W49" s="16"/>
+      <c r="X49" s="16"/>
+      <c r="Y49" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z49" s="16"/>
-      <c r="AA49" s="16"/>
-      <c r="AB49" s="16"/>
-      <c r="AC49" s="16"/>
+      <c r="Z49" s="15"/>
+      <c r="AA49" s="15"/>
+      <c r="AB49" s="15"/>
+      <c r="AC49" s="15"/>
       <c r="AD49" s="14" t="s">
         <v>1</v>
       </c>
@@ -7933,20 +8221,20 @@
       <c r="S50" s="4">
         <v>0</v>
       </c>
-      <c r="T50" s="15" t="s">
+      <c r="T50" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U50" s="15"/>
-      <c r="V50" s="15"/>
-      <c r="W50" s="15"/>
-      <c r="X50" s="15"/>
-      <c r="Y50" s="16" t="s">
+      <c r="U50" s="16"/>
+      <c r="V50" s="16"/>
+      <c r="W50" s="16"/>
+      <c r="X50" s="16"/>
+      <c r="Y50" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z50" s="16"/>
-      <c r="AA50" s="16"/>
-      <c r="AB50" s="16"/>
-      <c r="AC50" s="16"/>
+      <c r="Z50" s="15"/>
+      <c r="AA50" s="15"/>
+      <c r="AB50" s="15"/>
+      <c r="AC50" s="15"/>
       <c r="AD50" s="14" t="s">
         <v>75</v>
       </c>
@@ -8013,20 +8301,20 @@
       <c r="S51" s="4">
         <v>1</v>
       </c>
-      <c r="T51" s="15" t="s">
+      <c r="T51" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U51" s="15"/>
-      <c r="V51" s="15"/>
-      <c r="W51" s="15"/>
-      <c r="X51" s="15"/>
-      <c r="Y51" s="16" t="s">
+      <c r="U51" s="16"/>
+      <c r="V51" s="16"/>
+      <c r="W51" s="16"/>
+      <c r="X51" s="16"/>
+      <c r="Y51" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z51" s="16"/>
-      <c r="AA51" s="16"/>
-      <c r="AB51" s="16"/>
-      <c r="AC51" s="16"/>
+      <c r="Z51" s="15"/>
+      <c r="AA51" s="15"/>
+      <c r="AB51" s="15"/>
+      <c r="AC51" s="15"/>
       <c r="AD51" s="14" t="s">
         <v>75</v>
       </c>
@@ -8096,20 +8384,20 @@
       <c r="S52" s="4">
         <v>0</v>
       </c>
-      <c r="T52" s="15" t="s">
+      <c r="T52" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U52" s="15"/>
-      <c r="V52" s="15"/>
-      <c r="W52" s="15"/>
-      <c r="X52" s="15"/>
-      <c r="Y52" s="16" t="s">
+      <c r="U52" s="16"/>
+      <c r="V52" s="16"/>
+      <c r="W52" s="16"/>
+      <c r="X52" s="16"/>
+      <c r="Y52" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z52" s="16"/>
-      <c r="AA52" s="16"/>
-      <c r="AB52" s="16"/>
-      <c r="AC52" s="16"/>
+      <c r="Z52" s="15"/>
+      <c r="AA52" s="15"/>
+      <c r="AB52" s="15"/>
+      <c r="AC52" s="15"/>
       <c r="AD52" s="14" t="s">
         <v>1</v>
       </c>
@@ -8182,20 +8470,20 @@
       <c r="S53" s="4">
         <v>0</v>
       </c>
-      <c r="T53" s="15" t="s">
+      <c r="T53" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U53" s="15"/>
-      <c r="V53" s="15"/>
-      <c r="W53" s="15"/>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="16" t="s">
+      <c r="U53" s="16"/>
+      <c r="V53" s="16"/>
+      <c r="W53" s="16"/>
+      <c r="X53" s="16"/>
+      <c r="Y53" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z53" s="16"/>
-      <c r="AA53" s="16"/>
-      <c r="AB53" s="16"/>
-      <c r="AC53" s="16"/>
+      <c r="Z53" s="15"/>
+      <c r="AA53" s="15"/>
+      <c r="AB53" s="15"/>
+      <c r="AC53" s="15"/>
       <c r="AD53" s="14" t="s">
         <v>1</v>
       </c>
@@ -8268,20 +8556,20 @@
       <c r="S54" s="4">
         <v>1</v>
       </c>
-      <c r="T54" s="15" t="s">
+      <c r="T54" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U54" s="15"/>
-      <c r="V54" s="15"/>
-      <c r="W54" s="15"/>
-      <c r="X54" s="15"/>
-      <c r="Y54" s="16" t="s">
+      <c r="U54" s="16"/>
+      <c r="V54" s="16"/>
+      <c r="W54" s="16"/>
+      <c r="X54" s="16"/>
+      <c r="Y54" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z54" s="16"/>
-      <c r="AA54" s="16"/>
-      <c r="AB54" s="16"/>
-      <c r="AC54" s="16"/>
+      <c r="Z54" s="15"/>
+      <c r="AA54" s="15"/>
+      <c r="AB54" s="15"/>
+      <c r="AC54" s="15"/>
       <c r="AD54" s="14" t="s">
         <v>1</v>
       </c>
@@ -8354,20 +8642,20 @@
       <c r="S55" s="4">
         <v>0</v>
       </c>
-      <c r="T55" s="15" t="s">
+      <c r="T55" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U55" s="15"/>
-      <c r="V55" s="15"/>
-      <c r="W55" s="15"/>
-      <c r="X55" s="15"/>
-      <c r="Y55" s="16" t="s">
+      <c r="U55" s="16"/>
+      <c r="V55" s="16"/>
+      <c r="W55" s="16"/>
+      <c r="X55" s="16"/>
+      <c r="Y55" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z55" s="16"/>
-      <c r="AA55" s="16"/>
-      <c r="AB55" s="16"/>
-      <c r="AC55" s="16"/>
+      <c r="Z55" s="15"/>
+      <c r="AA55" s="15"/>
+      <c r="AB55" s="15"/>
+      <c r="AC55" s="15"/>
       <c r="AD55" s="14" t="s">
         <v>1</v>
       </c>
@@ -8434,20 +8722,20 @@
       <c r="S56" s="4">
         <v>1</v>
       </c>
-      <c r="T56" s="15" t="s">
+      <c r="T56" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U56" s="15"/>
-      <c r="V56" s="15"/>
-      <c r="W56" s="15"/>
-      <c r="X56" s="15"/>
-      <c r="Y56" s="16" t="s">
+      <c r="U56" s="16"/>
+      <c r="V56" s="16"/>
+      <c r="W56" s="16"/>
+      <c r="X56" s="16"/>
+      <c r="Y56" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z56" s="16"/>
-      <c r="AA56" s="16"/>
-      <c r="AB56" s="16"/>
-      <c r="AC56" s="16"/>
+      <c r="Z56" s="15"/>
+      <c r="AA56" s="15"/>
+      <c r="AB56" s="15"/>
+      <c r="AC56" s="15"/>
       <c r="AD56" s="14" t="s">
         <v>1</v>
       </c>
@@ -8514,20 +8802,20 @@
       <c r="S57" s="4">
         <v>0</v>
       </c>
-      <c r="T57" s="15" t="s">
+      <c r="T57" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U57" s="15"/>
-      <c r="V57" s="15"/>
-      <c r="W57" s="15"/>
-      <c r="X57" s="15"/>
-      <c r="Y57" s="16" t="s">
+      <c r="U57" s="16"/>
+      <c r="V57" s="16"/>
+      <c r="W57" s="16"/>
+      <c r="X57" s="16"/>
+      <c r="Y57" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z57" s="16"/>
-      <c r="AA57" s="16"/>
-      <c r="AB57" s="16"/>
-      <c r="AC57" s="16"/>
+      <c r="Z57" s="15"/>
+      <c r="AA57" s="15"/>
+      <c r="AB57" s="15"/>
+      <c r="AC57" s="15"/>
       <c r="AD57" s="14" t="s">
         <v>1</v>
       </c>
@@ -8594,20 +8882,20 @@
       <c r="S58" s="4">
         <v>1</v>
       </c>
-      <c r="T58" s="15" t="s">
+      <c r="T58" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U58" s="15"/>
-      <c r="V58" s="15"/>
-      <c r="W58" s="15"/>
-      <c r="X58" s="15"/>
-      <c r="Y58" s="16" t="s">
+      <c r="U58" s="16"/>
+      <c r="V58" s="16"/>
+      <c r="W58" s="16"/>
+      <c r="X58" s="16"/>
+      <c r="Y58" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z58" s="16"/>
-      <c r="AA58" s="16"/>
-      <c r="AB58" s="16"/>
-      <c r="AC58" s="16"/>
+      <c r="Z58" s="15"/>
+      <c r="AA58" s="15"/>
+      <c r="AB58" s="15"/>
+      <c r="AC58" s="15"/>
       <c r="AD58" s="14" t="s">
         <v>75</v>
       </c>
@@ -8674,20 +8962,20 @@
       <c r="S59" s="4">
         <v>0</v>
       </c>
-      <c r="T59" s="15" t="s">
+      <c r="T59" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U59" s="15"/>
-      <c r="V59" s="15"/>
-      <c r="W59" s="15"/>
-      <c r="X59" s="15"/>
-      <c r="Y59" s="16" t="s">
+      <c r="U59" s="16"/>
+      <c r="V59" s="16"/>
+      <c r="W59" s="16"/>
+      <c r="X59" s="16"/>
+      <c r="Y59" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z59" s="16"/>
-      <c r="AA59" s="16"/>
-      <c r="AB59" s="16"/>
-      <c r="AC59" s="16"/>
+      <c r="Z59" s="15"/>
+      <c r="AA59" s="15"/>
+      <c r="AB59" s="15"/>
+      <c r="AC59" s="15"/>
       <c r="AD59" s="14" t="s">
         <v>75</v>
       </c>
@@ -8754,20 +9042,20 @@
       <c r="S60" s="4">
         <v>1</v>
       </c>
-      <c r="T60" s="15" t="s">
+      <c r="T60" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U60" s="15"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="15"/>
-      <c r="X60" s="15"/>
-      <c r="Y60" s="16" t="s">
+      <c r="U60" s="16"/>
+      <c r="V60" s="16"/>
+      <c r="W60" s="16"/>
+      <c r="X60" s="16"/>
+      <c r="Y60" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z60" s="16"/>
-      <c r="AA60" s="16"/>
-      <c r="AB60" s="16"/>
-      <c r="AC60" s="16"/>
+      <c r="Z60" s="15"/>
+      <c r="AA60" s="15"/>
+      <c r="AB60" s="15"/>
+      <c r="AC60" s="15"/>
       <c r="AD60" s="14" t="s">
         <v>1</v>
       </c>
@@ -8834,20 +9122,20 @@
       <c r="S61" s="4">
         <v>0</v>
       </c>
-      <c r="T61" s="15" t="s">
+      <c r="T61" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U61" s="15"/>
-      <c r="V61" s="15"/>
-      <c r="W61" s="15"/>
-      <c r="X61" s="15"/>
-      <c r="Y61" s="16" t="s">
+      <c r="U61" s="16"/>
+      <c r="V61" s="16"/>
+      <c r="W61" s="16"/>
+      <c r="X61" s="16"/>
+      <c r="Y61" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z61" s="16"/>
-      <c r="AA61" s="16"/>
-      <c r="AB61" s="16"/>
-      <c r="AC61" s="16"/>
+      <c r="Z61" s="15"/>
+      <c r="AA61" s="15"/>
+      <c r="AB61" s="15"/>
+      <c r="AC61" s="15"/>
       <c r="AD61" s="14" t="s">
         <v>1</v>
       </c>
@@ -8914,20 +9202,20 @@
       <c r="S62" s="4">
         <v>1</v>
       </c>
-      <c r="T62" s="15" t="s">
+      <c r="T62" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U62" s="15"/>
-      <c r="V62" s="15"/>
-      <c r="W62" s="15"/>
-      <c r="X62" s="15"/>
-      <c r="Y62" s="16" t="s">
+      <c r="U62" s="16"/>
+      <c r="V62" s="16"/>
+      <c r="W62" s="16"/>
+      <c r="X62" s="16"/>
+      <c r="Y62" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z62" s="16"/>
-      <c r="AA62" s="16"/>
-      <c r="AB62" s="16"/>
-      <c r="AC62" s="16"/>
+      <c r="Z62" s="15"/>
+      <c r="AA62" s="15"/>
+      <c r="AB62" s="15"/>
+      <c r="AC62" s="15"/>
       <c r="AD62" s="14" t="s">
         <v>75</v>
       </c>
@@ -8994,20 +9282,20 @@
       <c r="S63" s="4">
         <v>0</v>
       </c>
-      <c r="T63" s="15" t="s">
+      <c r="T63" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U63" s="15"/>
-      <c r="V63" s="15"/>
-      <c r="W63" s="15"/>
-      <c r="X63" s="15"/>
-      <c r="Y63" s="16" t="s">
+      <c r="U63" s="16"/>
+      <c r="V63" s="16"/>
+      <c r="W63" s="16"/>
+      <c r="X63" s="16"/>
+      <c r="Y63" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z63" s="16"/>
-      <c r="AA63" s="16"/>
-      <c r="AB63" s="16"/>
-      <c r="AC63" s="16"/>
+      <c r="Z63" s="15"/>
+      <c r="AA63" s="15"/>
+      <c r="AB63" s="15"/>
+      <c r="AC63" s="15"/>
       <c r="AD63" s="14" t="s">
         <v>1</v>
       </c>
@@ -9074,20 +9362,20 @@
       <c r="S64" s="4">
         <v>1</v>
       </c>
-      <c r="T64" s="15" t="s">
+      <c r="T64" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U64" s="15"/>
-      <c r="V64" s="15"/>
-      <c r="W64" s="15"/>
-      <c r="X64" s="15"/>
-      <c r="Y64" s="16" t="s">
+      <c r="U64" s="16"/>
+      <c r="V64" s="16"/>
+      <c r="W64" s="16"/>
+      <c r="X64" s="16"/>
+      <c r="Y64" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z64" s="16"/>
-      <c r="AA64" s="16"/>
-      <c r="AB64" s="16"/>
-      <c r="AC64" s="16"/>
+      <c r="Z64" s="15"/>
+      <c r="AA64" s="15"/>
+      <c r="AB64" s="15"/>
+      <c r="AC64" s="15"/>
       <c r="AD64" s="14" t="s">
         <v>1</v>
       </c>
@@ -9154,20 +9442,20 @@
       <c r="S65" s="4">
         <v>0</v>
       </c>
-      <c r="T65" s="15" t="s">
+      <c r="T65" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="16" t="s">
+      <c r="U65" s="16"/>
+      <c r="V65" s="16"/>
+      <c r="W65" s="16"/>
+      <c r="X65" s="16"/>
+      <c r="Y65" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z65" s="16"/>
-      <c r="AA65" s="16"/>
-      <c r="AB65" s="16"/>
-      <c r="AC65" s="16"/>
+      <c r="Z65" s="15"/>
+      <c r="AA65" s="15"/>
+      <c r="AB65" s="15"/>
+      <c r="AC65" s="15"/>
       <c r="AD65" s="14" t="s">
         <v>1</v>
       </c>
@@ -9234,20 +9522,20 @@
       <c r="S66" s="4">
         <v>1</v>
       </c>
-      <c r="T66" s="15" t="s">
+      <c r="T66" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="15"/>
-      <c r="X66" s="15"/>
-      <c r="Y66" s="16" t="s">
+      <c r="U66" s="16"/>
+      <c r="V66" s="16"/>
+      <c r="W66" s="16"/>
+      <c r="X66" s="16"/>
+      <c r="Y66" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z66" s="16"/>
-      <c r="AA66" s="16"/>
-      <c r="AB66" s="16"/>
-      <c r="AC66" s="16"/>
+      <c r="Z66" s="15"/>
+      <c r="AA66" s="15"/>
+      <c r="AB66" s="15"/>
+      <c r="AC66" s="15"/>
       <c r="AD66" s="14" t="s">
         <v>1</v>
       </c>
@@ -9314,20 +9602,20 @@
       <c r="S67" s="4">
         <v>0</v>
       </c>
-      <c r="T67" s="15" t="s">
+      <c r="T67" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="U67" s="15"/>
-      <c r="V67" s="15"/>
-      <c r="W67" s="15"/>
-      <c r="X67" s="15"/>
-      <c r="Y67" s="16" t="s">
+      <c r="U67" s="16"/>
+      <c r="V67" s="16"/>
+      <c r="W67" s="16"/>
+      <c r="X67" s="16"/>
+      <c r="Y67" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z67" s="16"/>
-      <c r="AA67" s="16"/>
-      <c r="AB67" s="16"/>
-      <c r="AC67" s="16"/>
+      <c r="Z67" s="15"/>
+      <c r="AA67" s="15"/>
+      <c r="AB67" s="15"/>
+      <c r="AC67" s="15"/>
       <c r="AD67" s="14" t="s">
         <v>163</v>
       </c>
@@ -9388,20 +9676,20 @@
       <c r="S68" s="4">
         <v>1</v>
       </c>
-      <c r="T68" s="15" t="s">
+      <c r="T68" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="U68" s="15"/>
-      <c r="V68" s="15"/>
-      <c r="W68" s="15"/>
-      <c r="X68" s="15"/>
-      <c r="Y68" s="16" t="s">
+      <c r="U68" s="16"/>
+      <c r="V68" s="16"/>
+      <c r="W68" s="16"/>
+      <c r="X68" s="16"/>
+      <c r="Y68" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="Z68" s="16"/>
-      <c r="AA68" s="16"/>
-      <c r="AB68" s="16"/>
-      <c r="AC68" s="16"/>
+      <c r="Z68" s="15"/>
+      <c r="AA68" s="15"/>
+      <c r="AB68" s="15"/>
+      <c r="AC68" s="15"/>
       <c r="AD68" s="14" t="s">
         <v>75</v>
       </c>
@@ -9431,33 +9719,33 @@
       <c r="E70" s="5">
         <v>1</v>
       </c>
-      <c r="F70" s="16" t="s">
+      <c r="F70" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G70" s="16"/>
-      <c r="H70" s="16"/>
-      <c r="I70" s="16"/>
-      <c r="J70" s="16"/>
-      <c r="K70" s="16"/>
-      <c r="L70" s="16"/>
-      <c r="M70" s="16"/>
-      <c r="N70" s="16"/>
-      <c r="O70" s="16"/>
-      <c r="P70" s="16"/>
-      <c r="Q70" s="16"/>
-      <c r="R70" s="16"/>
-      <c r="S70" s="16"/>
-      <c r="T70" s="16"/>
-      <c r="U70" s="16"/>
-      <c r="V70" s="16"/>
-      <c r="W70" s="16"/>
-      <c r="X70" s="16"/>
-      <c r="Y70" s="16"/>
-      <c r="Z70" s="16"/>
-      <c r="AA70" s="16"/>
-      <c r="AB70" s="16"/>
-      <c r="AC70" s="16"/>
-      <c r="AD70" s="16"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="15"/>
+      <c r="X70" s="15"/>
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="15"/>
+      <c r="AA70" s="15"/>
+      <c r="AB70" s="15"/>
+      <c r="AC70" s="15"/>
+      <c r="AD70" s="15"/>
       <c r="AE70" s="14" t="s">
         <v>11</v>
       </c>
@@ -9484,33 +9772,33 @@
       <c r="E71" s="5">
         <v>0</v>
       </c>
-      <c r="F71" s="16" t="s">
+      <c r="F71" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
-      <c r="M71" s="16"/>
-      <c r="N71" s="16"/>
-      <c r="O71" s="16"/>
-      <c r="P71" s="16"/>
-      <c r="Q71" s="16"/>
-      <c r="R71" s="16"/>
-      <c r="S71" s="16"/>
-      <c r="T71" s="16"/>
-      <c r="U71" s="16"/>
-      <c r="V71" s="16"/>
-      <c r="W71" s="16"/>
-      <c r="X71" s="16"/>
-      <c r="Y71" s="16"/>
-      <c r="Z71" s="16"/>
-      <c r="AA71" s="16"/>
-      <c r="AB71" s="16"/>
-      <c r="AC71" s="16"/>
-      <c r="AD71" s="16"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="15"/>
+      <c r="X71" s="15"/>
+      <c r="Y71" s="15"/>
+      <c r="Z71" s="15"/>
+      <c r="AA71" s="15"/>
+      <c r="AB71" s="15"/>
+      <c r="AC71" s="15"/>
+      <c r="AD71" s="15"/>
       <c r="AE71" s="14" t="s">
         <v>11</v>
       </c>
@@ -9537,33 +9825,33 @@
       <c r="E72" s="5">
         <v>0</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F72" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G72" s="16"/>
-      <c r="H72" s="16"/>
-      <c r="I72" s="16"/>
-      <c r="J72" s="16"/>
-      <c r="K72" s="16"/>
-      <c r="L72" s="16"/>
-      <c r="M72" s="16"/>
-      <c r="N72" s="16"/>
-      <c r="O72" s="16"/>
-      <c r="P72" s="16"/>
-      <c r="Q72" s="16"/>
-      <c r="R72" s="16"/>
-      <c r="S72" s="16"/>
-      <c r="T72" s="16"/>
-      <c r="U72" s="16"/>
-      <c r="V72" s="16"/>
-      <c r="W72" s="16"/>
-      <c r="X72" s="16"/>
-      <c r="Y72" s="16"/>
-      <c r="Z72" s="16"/>
-      <c r="AA72" s="16"/>
-      <c r="AB72" s="16"/>
-      <c r="AC72" s="16"/>
-      <c r="AD72" s="16"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
+      <c r="Z72" s="15"/>
+      <c r="AA72" s="15"/>
+      <c r="AB72" s="15"/>
+      <c r="AC72" s="15"/>
+      <c r="AD72" s="15"/>
       <c r="AE72" s="14" t="s">
         <v>11</v>
       </c>
@@ -9591,33 +9879,33 @@
       <c r="E73" s="5">
         <v>1</v>
       </c>
-      <c r="F73" s="16" t="s">
+      <c r="F73" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G73" s="16"/>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
-      <c r="L73" s="16"/>
-      <c r="M73" s="16"/>
-      <c r="N73" s="16"/>
-      <c r="O73" s="16"/>
-      <c r="P73" s="16"/>
-      <c r="Q73" s="16"/>
-      <c r="R73" s="16"/>
-      <c r="S73" s="16"/>
-      <c r="T73" s="16"/>
-      <c r="U73" s="16"/>
-      <c r="V73" s="16"/>
-      <c r="W73" s="16"/>
-      <c r="X73" s="16"/>
-      <c r="Y73" s="16"/>
-      <c r="Z73" s="16"/>
-      <c r="AA73" s="16"/>
-      <c r="AB73" s="16"/>
-      <c r="AC73" s="16"/>
-      <c r="AD73" s="16"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+      <c r="AA73" s="15"/>
+      <c r="AB73" s="15"/>
+      <c r="AC73" s="15"/>
+      <c r="AD73" s="15"/>
       <c r="AE73" s="14" t="s">
         <v>11</v>
       </c>
@@ -9644,33 +9932,33 @@
       <c r="E74" s="5">
         <v>0</v>
       </c>
-      <c r="F74" s="16" t="s">
+      <c r="F74" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G74" s="16"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-      <c r="L74" s="16"/>
-      <c r="M74" s="16"/>
-      <c r="N74" s="16"/>
-      <c r="O74" s="16"/>
-      <c r="P74" s="16"/>
-      <c r="Q74" s="16"/>
-      <c r="R74" s="16"/>
-      <c r="S74" s="16"/>
-      <c r="T74" s="16"/>
-      <c r="U74" s="16"/>
-      <c r="V74" s="16"/>
-      <c r="W74" s="16"/>
-      <c r="X74" s="16"/>
-      <c r="Y74" s="16"/>
-      <c r="Z74" s="16"/>
-      <c r="AA74" s="16"/>
-      <c r="AB74" s="16"/>
-      <c r="AC74" s="16"/>
-      <c r="AD74" s="16"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
+      <c r="Z74" s="15"/>
+      <c r="AA74" s="15"/>
+      <c r="AB74" s="15"/>
+      <c r="AC74" s="15"/>
+      <c r="AD74" s="15"/>
       <c r="AE74" s="14" t="s">
         <v>11</v>
       </c>
@@ -9700,33 +9988,33 @@
       <c r="E75" s="5">
         <v>1</v>
       </c>
-      <c r="F75" s="16" t="s">
+      <c r="F75" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G75" s="16"/>
-      <c r="H75" s="16"/>
-      <c r="I75" s="16"/>
-      <c r="J75" s="16"/>
-      <c r="K75" s="16"/>
-      <c r="L75" s="16"/>
-      <c r="M75" s="16"/>
-      <c r="N75" s="16"/>
-      <c r="O75" s="16"/>
-      <c r="P75" s="16"/>
-      <c r="Q75" s="16"/>
-      <c r="R75" s="16"/>
-      <c r="S75" s="16"/>
-      <c r="T75" s="16"/>
-      <c r="U75" s="16"/>
-      <c r="V75" s="16"/>
-      <c r="W75" s="16"/>
-      <c r="X75" s="16"/>
-      <c r="Y75" s="16"/>
-      <c r="Z75" s="16"/>
-      <c r="AA75" s="16"/>
-      <c r="AB75" s="16"/>
-      <c r="AC75" s="16"/>
-      <c r="AD75" s="16"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="15"/>
+      <c r="X75" s="15"/>
+      <c r="Y75" s="15"/>
+      <c r="Z75" s="15"/>
+      <c r="AA75" s="15"/>
+      <c r="AB75" s="15"/>
+      <c r="AC75" s="15"/>
+      <c r="AD75" s="15"/>
       <c r="AE75" s="14" t="s">
         <v>11</v>
       </c>
@@ -9765,33 +10053,33 @@
       <c r="I76" s="1">
         <v>0</v>
       </c>
-      <c r="J76" s="16" t="s">
+      <c r="J76" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K76" s="16"/>
-      <c r="L76" s="16"/>
-      <c r="M76" s="16"/>
-      <c r="N76" s="16"/>
-      <c r="O76" s="16"/>
-      <c r="P76" s="16"/>
-      <c r="Q76" s="16"/>
-      <c r="R76" s="16"/>
-      <c r="S76" s="16"/>
-      <c r="T76" s="16"/>
-      <c r="U76" s="16"/>
-      <c r="V76" s="16"/>
-      <c r="W76" s="16"/>
-      <c r="X76" s="16"/>
-      <c r="Y76" s="16"/>
-      <c r="Z76" s="16"/>
-      <c r="AA76" s="16"/>
-      <c r="AB76" s="16"/>
-      <c r="AC76" s="16"/>
-      <c r="AD76" s="16"/>
-      <c r="AE76" s="16"/>
-      <c r="AF76" s="16"/>
-      <c r="AG76" s="16"/>
-      <c r="AH76" s="16"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="15"/>
+      <c r="X76" s="15"/>
+      <c r="Y76" s="15"/>
+      <c r="Z76" s="15"/>
+      <c r="AA76" s="15"/>
+      <c r="AB76" s="15"/>
+      <c r="AC76" s="15"/>
+      <c r="AD76" s="15"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
+      <c r="AH76" s="15"/>
       <c r="AI76" t="s">
         <v>165</v>
       </c>
@@ -9827,33 +10115,33 @@
       <c r="I77" s="1">
         <v>1</v>
       </c>
-      <c r="J77" s="16" t="s">
+      <c r="J77" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K77" s="16"/>
-      <c r="L77" s="16"/>
-      <c r="M77" s="16"/>
-      <c r="N77" s="16"/>
-      <c r="O77" s="16"/>
-      <c r="P77" s="16"/>
-      <c r="Q77" s="16"/>
-      <c r="R77" s="16"/>
-      <c r="S77" s="16"/>
-      <c r="T77" s="16"/>
-      <c r="U77" s="16"/>
-      <c r="V77" s="16"/>
-      <c r="W77" s="16"/>
-      <c r="X77" s="16"/>
-      <c r="Y77" s="16"/>
-      <c r="Z77" s="16"/>
-      <c r="AA77" s="16"/>
-      <c r="AB77" s="16"/>
-      <c r="AC77" s="16"/>
-      <c r="AD77" s="16"/>
-      <c r="AE77" s="16"/>
-      <c r="AF77" s="16"/>
-      <c r="AG77" s="16"/>
-      <c r="AH77" s="16"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="15"/>
+      <c r="X77" s="15"/>
+      <c r="Y77" s="15"/>
+      <c r="Z77" s="15"/>
+      <c r="AA77" s="15"/>
+      <c r="AB77" s="15"/>
+      <c r="AC77" s="15"/>
+      <c r="AD77" s="15"/>
+      <c r="AE77" s="15"/>
+      <c r="AF77" s="15"/>
+      <c r="AG77" s="15"/>
+      <c r="AH77" s="15"/>
       <c r="AI77" t="s">
         <v>167</v>
       </c>
@@ -9889,26 +10177,26 @@
       <c r="J80" s="1">
         <v>0</v>
       </c>
-      <c r="K80" s="15" t="s">
+      <c r="K80" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
-      <c r="O80" s="15"/>
-      <c r="P80" s="15"/>
-      <c r="Q80" s="15"/>
-      <c r="R80" s="15"/>
-      <c r="S80" s="16" t="s">
+      <c r="L80" s="16"/>
+      <c r="M80" s="16"/>
+      <c r="N80" s="16"/>
+      <c r="O80" s="16"/>
+      <c r="P80" s="16"/>
+      <c r="Q80" s="16"/>
+      <c r="R80" s="16"/>
+      <c r="S80" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T80" s="16"/>
-      <c r="U80" s="16"/>
-      <c r="V80" s="16"/>
-      <c r="W80" s="16"/>
-      <c r="X80" s="16"/>
-      <c r="Y80" s="16"/>
-      <c r="Z80" s="16"/>
+      <c r="T80" s="15"/>
+      <c r="U80" s="15"/>
+      <c r="V80" s="15"/>
+      <c r="W80" s="15"/>
+      <c r="X80" s="15"/>
+      <c r="Y80" s="15"/>
+      <c r="Z80" s="15"/>
       <c r="AA80" s="14" t="s">
         <v>11</v>
       </c>
@@ -9960,26 +10248,26 @@
       <c r="J81" s="4">
         <v>1</v>
       </c>
-      <c r="K81" s="15" t="s">
+      <c r="K81" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
-      <c r="O81" s="15"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
-      <c r="R81" s="15"/>
-      <c r="S81" s="16" t="s">
+      <c r="L81" s="16"/>
+      <c r="M81" s="16"/>
+      <c r="N81" s="16"/>
+      <c r="O81" s="16"/>
+      <c r="P81" s="16"/>
+      <c r="Q81" s="16"/>
+      <c r="R81" s="16"/>
+      <c r="S81" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T81" s="16"/>
-      <c r="U81" s="16"/>
-      <c r="V81" s="16"/>
-      <c r="W81" s="16"/>
-      <c r="X81" s="16"/>
-      <c r="Y81" s="16"/>
-      <c r="Z81" s="16"/>
+      <c r="T81" s="15"/>
+      <c r="U81" s="15"/>
+      <c r="V81" s="15"/>
+      <c r="W81" s="15"/>
+      <c r="X81" s="15"/>
+      <c r="Y81" s="15"/>
+      <c r="Z81" s="15"/>
       <c r="AA81" s="14" t="s">
         <v>11</v>
       </c>
@@ -10031,26 +10319,26 @@
       <c r="J82" s="4">
         <v>0</v>
       </c>
-      <c r="K82" s="15" t="s">
+      <c r="K82" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L82" s="15"/>
-      <c r="M82" s="15"/>
-      <c r="N82" s="15"/>
-      <c r="O82" s="15"/>
-      <c r="P82" s="15"/>
-      <c r="Q82" s="15"/>
-      <c r="R82" s="15"/>
-      <c r="S82" s="16" t="s">
+      <c r="L82" s="16"/>
+      <c r="M82" s="16"/>
+      <c r="N82" s="16"/>
+      <c r="O82" s="16"/>
+      <c r="P82" s="16"/>
+      <c r="Q82" s="16"/>
+      <c r="R82" s="16"/>
+      <c r="S82" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T82" s="16"/>
-      <c r="U82" s="16"/>
-      <c r="V82" s="16"/>
-      <c r="W82" s="16"/>
-      <c r="X82" s="16"/>
-      <c r="Y82" s="16"/>
-      <c r="Z82" s="16"/>
+      <c r="T82" s="15"/>
+      <c r="U82" s="15"/>
+      <c r="V82" s="15"/>
+      <c r="W82" s="15"/>
+      <c r="X82" s="15"/>
+      <c r="Y82" s="15"/>
+      <c r="Z82" s="15"/>
       <c r="AA82" s="14" t="s">
         <v>11</v>
       </c>
@@ -10102,26 +10390,26 @@
       <c r="J83" s="4">
         <v>1</v>
       </c>
-      <c r="K83" s="15" t="s">
+      <c r="K83" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L83" s="15"/>
-      <c r="M83" s="15"/>
-      <c r="N83" s="15"/>
-      <c r="O83" s="15"/>
-      <c r="P83" s="15"/>
-      <c r="Q83" s="15"/>
-      <c r="R83" s="15"/>
-      <c r="S83" s="16" t="s">
+      <c r="L83" s="16"/>
+      <c r="M83" s="16"/>
+      <c r="N83" s="16"/>
+      <c r="O83" s="16"/>
+      <c r="P83" s="16"/>
+      <c r="Q83" s="16"/>
+      <c r="R83" s="16"/>
+      <c r="S83" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T83" s="16"/>
-      <c r="U83" s="16"/>
-      <c r="V83" s="16"/>
-      <c r="W83" s="16"/>
-      <c r="X83" s="16"/>
-      <c r="Y83" s="16"/>
-      <c r="Z83" s="16"/>
+      <c r="T83" s="15"/>
+      <c r="U83" s="15"/>
+      <c r="V83" s="15"/>
+      <c r="W83" s="15"/>
+      <c r="X83" s="15"/>
+      <c r="Y83" s="15"/>
+      <c r="Z83" s="15"/>
       <c r="AA83" s="14" t="s">
         <v>11</v>
       </c>
@@ -10176,26 +10464,26 @@
       <c r="J84" s="4">
         <v>0</v>
       </c>
-      <c r="K84" s="15" t="s">
+      <c r="K84" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L84" s="15"/>
-      <c r="M84" s="15"/>
-      <c r="N84" s="15"/>
-      <c r="O84" s="15"/>
-      <c r="P84" s="15"/>
-      <c r="Q84" s="15"/>
-      <c r="R84" s="15"/>
-      <c r="S84" s="16" t="s">
+      <c r="L84" s="16"/>
+      <c r="M84" s="16"/>
+      <c r="N84" s="16"/>
+      <c r="O84" s="16"/>
+      <c r="P84" s="16"/>
+      <c r="Q84" s="16"/>
+      <c r="R84" s="16"/>
+      <c r="S84" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T84" s="16"/>
-      <c r="U84" s="16"/>
-      <c r="V84" s="16"/>
-      <c r="W84" s="16"/>
-      <c r="X84" s="16"/>
-      <c r="Y84" s="16"/>
-      <c r="Z84" s="16"/>
+      <c r="T84" s="15"/>
+      <c r="U84" s="15"/>
+      <c r="V84" s="15"/>
+      <c r="W84" s="15"/>
+      <c r="X84" s="15"/>
+      <c r="Y84" s="15"/>
+      <c r="Z84" s="15"/>
       <c r="AA84" s="14" t="s">
         <v>11</v>
       </c>
@@ -10247,26 +10535,26 @@
       <c r="J85" s="4">
         <v>1</v>
       </c>
-      <c r="K85" s="15" t="s">
+      <c r="K85" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L85" s="15"/>
-      <c r="M85" s="15"/>
-      <c r="N85" s="15"/>
-      <c r="O85" s="15"/>
-      <c r="P85" s="15"/>
-      <c r="Q85" s="15"/>
-      <c r="R85" s="15"/>
-      <c r="S85" s="16" t="s">
+      <c r="L85" s="16"/>
+      <c r="M85" s="16"/>
+      <c r="N85" s="16"/>
+      <c r="O85" s="16"/>
+      <c r="P85" s="16"/>
+      <c r="Q85" s="16"/>
+      <c r="R85" s="16"/>
+      <c r="S85" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T85" s="16"/>
-      <c r="U85" s="16"/>
-      <c r="V85" s="16"/>
-      <c r="W85" s="16"/>
-      <c r="X85" s="16"/>
-      <c r="Y85" s="16"/>
-      <c r="Z85" s="16"/>
+      <c r="T85" s="15"/>
+      <c r="U85" s="15"/>
+      <c r="V85" s="15"/>
+      <c r="W85" s="15"/>
+      <c r="X85" s="15"/>
+      <c r="Y85" s="15"/>
+      <c r="Z85" s="15"/>
       <c r="AA85" s="14" t="s">
         <v>11</v>
       </c>
@@ -10318,26 +10606,26 @@
       <c r="J86" s="4">
         <v>0</v>
       </c>
-      <c r="K86" s="15" t="s">
+      <c r="K86" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L86" s="15"/>
-      <c r="M86" s="15"/>
-      <c r="N86" s="15"/>
-      <c r="O86" s="15"/>
-      <c r="P86" s="15"/>
-      <c r="Q86" s="15"/>
-      <c r="R86" s="15"/>
-      <c r="S86" s="16" t="s">
+      <c r="L86" s="16"/>
+      <c r="M86" s="16"/>
+      <c r="N86" s="16"/>
+      <c r="O86" s="16"/>
+      <c r="P86" s="16"/>
+      <c r="Q86" s="16"/>
+      <c r="R86" s="16"/>
+      <c r="S86" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T86" s="16"/>
-      <c r="U86" s="16"/>
-      <c r="V86" s="16"/>
-      <c r="W86" s="16"/>
-      <c r="X86" s="16"/>
-      <c r="Y86" s="16"/>
-      <c r="Z86" s="16"/>
+      <c r="T86" s="15"/>
+      <c r="U86" s="15"/>
+      <c r="V86" s="15"/>
+      <c r="W86" s="15"/>
+      <c r="X86" s="15"/>
+      <c r="Y86" s="15"/>
+      <c r="Z86" s="15"/>
       <c r="AA86" s="14" t="s">
         <v>11</v>
       </c>
@@ -10389,26 +10677,26 @@
       <c r="J87" s="4">
         <v>1</v>
       </c>
-      <c r="K87" s="15" t="s">
+      <c r="K87" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L87" s="15"/>
-      <c r="M87" s="15"/>
-      <c r="N87" s="15"/>
-      <c r="O87" s="15"/>
-      <c r="P87" s="15"/>
-      <c r="Q87" s="15"/>
-      <c r="R87" s="15"/>
-      <c r="S87" s="16" t="s">
+      <c r="L87" s="16"/>
+      <c r="M87" s="16"/>
+      <c r="N87" s="16"/>
+      <c r="O87" s="16"/>
+      <c r="P87" s="16"/>
+      <c r="Q87" s="16"/>
+      <c r="R87" s="16"/>
+      <c r="S87" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T87" s="16"/>
-      <c r="U87" s="16"/>
-      <c r="V87" s="16"/>
-      <c r="W87" s="16"/>
-      <c r="X87" s="16"/>
-      <c r="Y87" s="16"/>
-      <c r="Z87" s="16"/>
+      <c r="T87" s="15"/>
+      <c r="U87" s="15"/>
+      <c r="V87" s="15"/>
+      <c r="W87" s="15"/>
+      <c r="X87" s="15"/>
+      <c r="Y87" s="15"/>
+      <c r="Z87" s="15"/>
       <c r="AA87" s="14" t="s">
         <v>11</v>
       </c>
@@ -10483,16 +10771,16 @@
       <c r="R90" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="S90" s="16" t="s">
+      <c r="S90" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T90" s="16"/>
-      <c r="U90" s="16"/>
-      <c r="V90" s="16"/>
-      <c r="W90" s="16"/>
-      <c r="X90" s="16"/>
-      <c r="Y90" s="16"/>
-      <c r="Z90" s="16"/>
+      <c r="T90" s="15"/>
+      <c r="U90" s="15"/>
+      <c r="V90" s="15"/>
+      <c r="W90" s="15"/>
+      <c r="X90" s="15"/>
+      <c r="Y90" s="15"/>
+      <c r="Z90" s="15"/>
       <c r="AA90" s="14" t="s">
         <v>11</v>
       </c>
@@ -10559,16 +10847,16 @@
       <c r="R91" s="4">
         <v>0</v>
       </c>
-      <c r="S91" s="16" t="s">
+      <c r="S91" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T91" s="16"/>
-      <c r="U91" s="16"/>
-      <c r="V91" s="16"/>
-      <c r="W91" s="16"/>
-      <c r="X91" s="16"/>
-      <c r="Y91" s="16"/>
-      <c r="Z91" s="16"/>
+      <c r="T91" s="15"/>
+      <c r="U91" s="15"/>
+      <c r="V91" s="15"/>
+      <c r="W91" s="15"/>
+      <c r="X91" s="15"/>
+      <c r="Y91" s="15"/>
+      <c r="Z91" s="15"/>
       <c r="AA91" s="14" t="s">
         <v>11</v>
       </c>
@@ -10641,16 +10929,16 @@
       <c r="R92" s="4">
         <v>1</v>
       </c>
-      <c r="S92" s="16" t="s">
+      <c r="S92" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T92" s="16"/>
-      <c r="U92" s="16"/>
-      <c r="V92" s="16"/>
-      <c r="W92" s="16"/>
-      <c r="X92" s="16"/>
-      <c r="Y92" s="16"/>
-      <c r="Z92" s="16"/>
+      <c r="T92" s="15"/>
+      <c r="U92" s="15"/>
+      <c r="V92" s="15"/>
+      <c r="W92" s="15"/>
+      <c r="X92" s="15"/>
+      <c r="Y92" s="15"/>
+      <c r="Z92" s="15"/>
       <c r="AA92" s="14" t="s">
         <v>11</v>
       </c>
@@ -10723,16 +11011,16 @@
       <c r="R93" s="4">
         <v>0</v>
       </c>
-      <c r="S93" s="16" t="s">
+      <c r="S93" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T93" s="16"/>
-      <c r="U93" s="16"/>
-      <c r="V93" s="16"/>
-      <c r="W93" s="16"/>
-      <c r="X93" s="16"/>
-      <c r="Y93" s="16"/>
-      <c r="Z93" s="16"/>
+      <c r="T93" s="15"/>
+      <c r="U93" s="15"/>
+      <c r="V93" s="15"/>
+      <c r="W93" s="15"/>
+      <c r="X93" s="15"/>
+      <c r="Y93" s="15"/>
+      <c r="Z93" s="15"/>
       <c r="AA93" s="14" t="s">
         <v>11</v>
       </c>
@@ -10805,16 +11093,16 @@
       <c r="R94" s="4">
         <v>1</v>
       </c>
-      <c r="S94" s="16" t="s">
+      <c r="S94" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="T94" s="16"/>
-      <c r="U94" s="16"/>
-      <c r="V94" s="16"/>
-      <c r="W94" s="16"/>
-      <c r="X94" s="16"/>
-      <c r="Y94" s="16"/>
-      <c r="Z94" s="16"/>
+      <c r="T94" s="15"/>
+      <c r="U94" s="15"/>
+      <c r="V94" s="15"/>
+      <c r="W94" s="15"/>
+      <c r="X94" s="15"/>
+      <c r="Y94" s="15"/>
+      <c r="Z94" s="15"/>
       <c r="AA94" s="14" t="s">
         <v>11</v>
       </c>
@@ -10887,16 +11175,16 @@
       <c r="R95" s="4">
         <v>0</v>
       </c>
-      <c r="S95" s="16" t="s">
+      <c r="S95" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="T95" s="16"/>
-      <c r="U95" s="16"/>
-      <c r="V95" s="16"/>
-      <c r="W95" s="16"/>
-      <c r="X95" s="16"/>
-      <c r="Y95" s="16"/>
-      <c r="Z95" s="16"/>
+      <c r="T95" s="15"/>
+      <c r="U95" s="15"/>
+      <c r="V95" s="15"/>
+      <c r="W95" s="15"/>
+      <c r="X95" s="15"/>
+      <c r="Y95" s="15"/>
+      <c r="Z95" s="15"/>
       <c r="AA95" s="14" t="s">
         <v>11</v>
       </c>
@@ -10969,16 +11257,16 @@
       <c r="R96" s="4">
         <v>1</v>
       </c>
-      <c r="S96" s="16" t="s">
+      <c r="S96" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="T96" s="16"/>
-      <c r="U96" s="16"/>
-      <c r="V96" s="16"/>
-      <c r="W96" s="16"/>
-      <c r="X96" s="16"/>
-      <c r="Y96" s="16"/>
-      <c r="Z96" s="16"/>
+      <c r="T96" s="15"/>
+      <c r="U96" s="15"/>
+      <c r="V96" s="15"/>
+      <c r="W96" s="15"/>
+      <c r="X96" s="15"/>
+      <c r="Y96" s="15"/>
+      <c r="Z96" s="15"/>
       <c r="AA96" s="14" t="s">
         <v>75</v>
       </c>
@@ -11048,16 +11336,16 @@
       <c r="R97" s="4">
         <v>0</v>
       </c>
-      <c r="S97" s="16" t="s">
+      <c r="S97" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T97" s="16"/>
-      <c r="U97" s="16"/>
-      <c r="V97" s="16"/>
-      <c r="W97" s="16"/>
-      <c r="X97" s="16"/>
-      <c r="Y97" s="16"/>
-      <c r="Z97" s="16"/>
+      <c r="T97" s="15"/>
+      <c r="U97" s="15"/>
+      <c r="V97" s="15"/>
+      <c r="W97" s="15"/>
+      <c r="X97" s="15"/>
+      <c r="Y97" s="15"/>
+      <c r="Z97" s="15"/>
       <c r="AA97" s="14" t="s">
         <v>75</v>
       </c>
@@ -11127,16 +11415,16 @@
       <c r="R98" s="4">
         <v>1</v>
       </c>
-      <c r="S98" s="16" t="s">
+      <c r="S98" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T98" s="16"/>
-      <c r="U98" s="16"/>
-      <c r="V98" s="16"/>
-      <c r="W98" s="16"/>
-      <c r="X98" s="16"/>
-      <c r="Y98" s="16"/>
-      <c r="Z98" s="16"/>
+      <c r="T98" s="15"/>
+      <c r="U98" s="15"/>
+      <c r="V98" s="15"/>
+      <c r="W98" s="15"/>
+      <c r="X98" s="15"/>
+      <c r="Y98" s="15"/>
+      <c r="Z98" s="15"/>
       <c r="AA98" s="14" t="s">
         <v>11</v>
       </c>
@@ -11209,16 +11497,16 @@
       <c r="R99" s="4">
         <v>0</v>
       </c>
-      <c r="S99" s="16" t="s">
+      <c r="S99" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="T99" s="16"/>
-      <c r="U99" s="16"/>
-      <c r="V99" s="16"/>
-      <c r="W99" s="16"/>
-      <c r="X99" s="16"/>
-      <c r="Y99" s="16"/>
-      <c r="Z99" s="16"/>
+      <c r="T99" s="15"/>
+      <c r="U99" s="15"/>
+      <c r="V99" s="15"/>
+      <c r="W99" s="15"/>
+      <c r="X99" s="15"/>
+      <c r="Y99" s="15"/>
+      <c r="Z99" s="15"/>
       <c r="AA99" s="14" t="s">
         <v>11</v>
       </c>
@@ -11291,16 +11579,16 @@
       <c r="R100" s="4">
         <v>1</v>
       </c>
-      <c r="S100" s="16" t="s">
+      <c r="S100" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="T100" s="16"/>
-      <c r="U100" s="16"/>
-      <c r="V100" s="16"/>
-      <c r="W100" s="16"/>
-      <c r="X100" s="16"/>
-      <c r="Y100" s="16"/>
-      <c r="Z100" s="16"/>
+      <c r="T100" s="15"/>
+      <c r="U100" s="15"/>
+      <c r="V100" s="15"/>
+      <c r="W100" s="15"/>
+      <c r="X100" s="15"/>
+      <c r="Y100" s="15"/>
+      <c r="Z100" s="15"/>
       <c r="AA100" s="14" t="s">
         <v>11</v>
       </c>
@@ -11373,16 +11661,16 @@
       <c r="R101" s="4">
         <v>0</v>
       </c>
-      <c r="S101" s="16" t="s">
+      <c r="S101" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T101" s="16"/>
-      <c r="U101" s="16"/>
-      <c r="V101" s="16"/>
-      <c r="W101" s="16"/>
-      <c r="X101" s="16"/>
-      <c r="Y101" s="16"/>
-      <c r="Z101" s="16"/>
+      <c r="T101" s="15"/>
+      <c r="U101" s="15"/>
+      <c r="V101" s="15"/>
+      <c r="W101" s="15"/>
+      <c r="X101" s="15"/>
+      <c r="Y101" s="15"/>
+      <c r="Z101" s="15"/>
       <c r="AA101" s="14" t="s">
         <v>11</v>
       </c>
@@ -11455,16 +11743,16 @@
       <c r="R102" s="4">
         <v>1</v>
       </c>
-      <c r="S102" s="16" t="s">
+      <c r="S102" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T102" s="16"/>
-      <c r="U102" s="16"/>
-      <c r="V102" s="16"/>
-      <c r="W102" s="16"/>
-      <c r="X102" s="16"/>
-      <c r="Y102" s="16"/>
-      <c r="Z102" s="16"/>
+      <c r="T102" s="15"/>
+      <c r="U102" s="15"/>
+      <c r="V102" s="15"/>
+      <c r="W102" s="15"/>
+      <c r="X102" s="15"/>
+      <c r="Y102" s="15"/>
+      <c r="Z102" s="15"/>
       <c r="AA102" s="14" t="s">
         <v>11</v>
       </c>
@@ -11537,16 +11825,16 @@
       <c r="R103" s="4">
         <v>0</v>
       </c>
-      <c r="S103" s="16" t="s">
+      <c r="S103" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T103" s="16"/>
-      <c r="U103" s="16"/>
-      <c r="V103" s="16"/>
-      <c r="W103" s="16"/>
-      <c r="X103" s="16"/>
-      <c r="Y103" s="16"/>
-      <c r="Z103" s="16"/>
+      <c r="T103" s="15"/>
+      <c r="U103" s="15"/>
+      <c r="V103" s="15"/>
+      <c r="W103" s="15"/>
+      <c r="X103" s="15"/>
+      <c r="Y103" s="15"/>
+      <c r="Z103" s="15"/>
       <c r="AA103" s="14" t="s">
         <v>11</v>
       </c>
@@ -11620,16 +11908,16 @@
       <c r="R104" s="4">
         <v>1</v>
       </c>
-      <c r="S104" s="16" t="s">
+      <c r="S104" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T104" s="16"/>
-      <c r="U104" s="16"/>
-      <c r="V104" s="16"/>
-      <c r="W104" s="16"/>
-      <c r="X104" s="16"/>
-      <c r="Y104" s="16"/>
-      <c r="Z104" s="16"/>
+      <c r="T104" s="15"/>
+      <c r="U104" s="15"/>
+      <c r="V104" s="15"/>
+      <c r="W104" s="15"/>
+      <c r="X104" s="15"/>
+      <c r="Y104" s="15"/>
+      <c r="Z104" s="15"/>
       <c r="AA104" s="14" t="s">
         <v>11</v>
       </c>
@@ -11730,24 +12018,24 @@
       <c r="M108" s="3">
         <v>1</v>
       </c>
-      <c r="N108" s="16" t="s">
+      <c r="N108" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="O108" s="16"/>
-      <c r="P108" s="16"/>
-      <c r="Q108" s="16"/>
-      <c r="R108" s="16"/>
-      <c r="S108" s="16"/>
-      <c r="T108" s="16"/>
-      <c r="U108" s="16"/>
-      <c r="V108" s="16"/>
-      <c r="W108" s="16"/>
-      <c r="X108" s="16"/>
-      <c r="Y108" s="16"/>
-      <c r="Z108" s="16"/>
-      <c r="AA108" s="16"/>
-      <c r="AB108" s="16"/>
-      <c r="AC108" s="16"/>
+      <c r="O108" s="15"/>
+      <c r="P108" s="15"/>
+      <c r="Q108" s="15"/>
+      <c r="R108" s="15"/>
+      <c r="S108" s="15"/>
+      <c r="T108" s="15"/>
+      <c r="U108" s="15"/>
+      <c r="V108" s="15"/>
+      <c r="W108" s="15"/>
+      <c r="X108" s="15"/>
+      <c r="Y108" s="15"/>
+      <c r="Z108" s="15"/>
+      <c r="AA108" s="15"/>
+      <c r="AB108" s="15"/>
+      <c r="AC108" s="15"/>
       <c r="AD108" s="17" t="s">
         <v>1</v>
       </c>
@@ -11796,24 +12084,24 @@
       <c r="M109" s="3">
         <v>1</v>
       </c>
-      <c r="N109" s="16" t="s">
+      <c r="N109" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="O109" s="16"/>
-      <c r="P109" s="16"/>
-      <c r="Q109" s="16"/>
-      <c r="R109" s="16"/>
-      <c r="S109" s="16"/>
-      <c r="T109" s="16"/>
-      <c r="U109" s="16"/>
-      <c r="V109" s="16"/>
-      <c r="W109" s="16"/>
-      <c r="X109" s="16"/>
-      <c r="Y109" s="16"/>
-      <c r="Z109" s="16"/>
-      <c r="AA109" s="16"/>
-      <c r="AB109" s="16"/>
-      <c r="AC109" s="16"/>
+      <c r="O109" s="15"/>
+      <c r="P109" s="15"/>
+      <c r="Q109" s="15"/>
+      <c r="R109" s="15"/>
+      <c r="S109" s="15"/>
+      <c r="T109" s="15"/>
+      <c r="U109" s="15"/>
+      <c r="V109" s="15"/>
+      <c r="W109" s="15"/>
+      <c r="X109" s="15"/>
+      <c r="Y109" s="15"/>
+      <c r="Z109" s="15"/>
+      <c r="AA109" s="15"/>
+      <c r="AB109" s="15"/>
+      <c r="AC109" s="15"/>
       <c r="AD109" s="17" t="s">
         <v>1</v>
       </c>
@@ -11824,70 +12112,191 @@
     </row>
   </sheetData>
   <mergeCells count="273">
-    <mergeCell ref="C107:M107"/>
-    <mergeCell ref="N107:AC107"/>
-    <mergeCell ref="AD107:AH107"/>
-    <mergeCell ref="AA99:AH99"/>
-    <mergeCell ref="AA100:AH100"/>
-    <mergeCell ref="AA101:AH101"/>
-    <mergeCell ref="AA102:AH102"/>
-    <mergeCell ref="AA103:AH103"/>
-    <mergeCell ref="AA104:AH104"/>
-    <mergeCell ref="S103:Z103"/>
-    <mergeCell ref="S104:Z104"/>
-    <mergeCell ref="S99:Z99"/>
-    <mergeCell ref="S100:Z100"/>
-    <mergeCell ref="S101:Z101"/>
-    <mergeCell ref="S102:Z102"/>
-    <mergeCell ref="AA91:AH91"/>
-    <mergeCell ref="AA92:AH92"/>
-    <mergeCell ref="AA93:AH93"/>
-    <mergeCell ref="AA94:AH94"/>
-    <mergeCell ref="AA95:AH95"/>
-    <mergeCell ref="AA96:AH96"/>
-    <mergeCell ref="AA97:AH97"/>
-    <mergeCell ref="AA98:AH98"/>
-    <mergeCell ref="S97:Z97"/>
-    <mergeCell ref="S98:Z98"/>
-    <mergeCell ref="S91:Z91"/>
-    <mergeCell ref="S92:Z92"/>
-    <mergeCell ref="S93:Z93"/>
-    <mergeCell ref="S94:Z94"/>
-    <mergeCell ref="S95:Z95"/>
-    <mergeCell ref="S96:Z96"/>
-    <mergeCell ref="K87:R87"/>
-    <mergeCell ref="S81:Z81"/>
-    <mergeCell ref="S82:Z82"/>
-    <mergeCell ref="S83:Z83"/>
-    <mergeCell ref="S84:Z84"/>
-    <mergeCell ref="S85:Z85"/>
-    <mergeCell ref="S90:Z90"/>
-    <mergeCell ref="AA90:AH90"/>
-    <mergeCell ref="S87:Z87"/>
-    <mergeCell ref="AA81:AH81"/>
-    <mergeCell ref="AA82:AH82"/>
-    <mergeCell ref="AA83:AH83"/>
-    <mergeCell ref="AA84:AH84"/>
-    <mergeCell ref="AA85:AH85"/>
-    <mergeCell ref="AA86:AH86"/>
-    <mergeCell ref="AA87:AH87"/>
-    <mergeCell ref="S86:Z86"/>
-    <mergeCell ref="J77:AH77"/>
-    <mergeCell ref="T68:X68"/>
-    <mergeCell ref="Y68:AC68"/>
-    <mergeCell ref="AD68:AH68"/>
-    <mergeCell ref="K84:R84"/>
-    <mergeCell ref="K85:R85"/>
-    <mergeCell ref="K86:R86"/>
-    <mergeCell ref="J76:AH76"/>
-    <mergeCell ref="AE74:AH74"/>
-    <mergeCell ref="AE75:AH75"/>
-    <mergeCell ref="F72:AD72"/>
-    <mergeCell ref="F73:AD73"/>
-    <mergeCell ref="F74:AD74"/>
-    <mergeCell ref="F75:AD75"/>
-    <mergeCell ref="AE71:AH71"/>
-    <mergeCell ref="AE72:AH72"/>
+    <mergeCell ref="AD15:AH15"/>
+    <mergeCell ref="T16:X16"/>
+    <mergeCell ref="Y16:AC16"/>
+    <mergeCell ref="T13:X13"/>
+    <mergeCell ref="Y13:AC13"/>
+    <mergeCell ref="AD13:AH13"/>
+    <mergeCell ref="N108:AC108"/>
+    <mergeCell ref="AD108:AH108"/>
+    <mergeCell ref="N109:AC109"/>
+    <mergeCell ref="AD109:AH109"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="Y17:AC17"/>
+    <mergeCell ref="AD17:AH17"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="Y18:AC18"/>
+    <mergeCell ref="AD18:AH18"/>
+    <mergeCell ref="T15:X15"/>
+    <mergeCell ref="Y15:AC15"/>
+    <mergeCell ref="AD16:AH16"/>
+    <mergeCell ref="T21:X21"/>
+    <mergeCell ref="Y21:AC21"/>
+    <mergeCell ref="AD21:AH21"/>
+    <mergeCell ref="T22:X22"/>
+    <mergeCell ref="Y22:AC22"/>
+    <mergeCell ref="T7:X7"/>
+    <mergeCell ref="Y7:AC7"/>
+    <mergeCell ref="AD7:AH7"/>
+    <mergeCell ref="T8:X8"/>
+    <mergeCell ref="Y8:AC8"/>
+    <mergeCell ref="AD8:AH8"/>
+    <mergeCell ref="T14:X14"/>
+    <mergeCell ref="Y14:AC14"/>
+    <mergeCell ref="AD14:AH14"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="Y3:AC3"/>
+    <mergeCell ref="AD3:AH3"/>
+    <mergeCell ref="T12:X12"/>
+    <mergeCell ref="Y12:AC12"/>
+    <mergeCell ref="AD12:AH12"/>
+    <mergeCell ref="T10:X10"/>
+    <mergeCell ref="Y10:AC10"/>
+    <mergeCell ref="AD10:AH10"/>
+    <mergeCell ref="T11:X11"/>
+    <mergeCell ref="Y11:AC11"/>
+    <mergeCell ref="AD11:AH11"/>
+    <mergeCell ref="T9:X9"/>
+    <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="AD9:AH9"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="AD5:AH5"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="Y4:AC4"/>
+    <mergeCell ref="AD4:AH4"/>
+    <mergeCell ref="T6:X6"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AD6:AH6"/>
+    <mergeCell ref="AD22:AH22"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="Y19:AC19"/>
+    <mergeCell ref="AD19:AH19"/>
+    <mergeCell ref="T20:X20"/>
+    <mergeCell ref="Y20:AC20"/>
+    <mergeCell ref="AD20:AH20"/>
+    <mergeCell ref="T25:X25"/>
+    <mergeCell ref="Y25:AC25"/>
+    <mergeCell ref="AD25:AH25"/>
+    <mergeCell ref="T26:X26"/>
+    <mergeCell ref="Y26:AC26"/>
+    <mergeCell ref="AD26:AH26"/>
+    <mergeCell ref="T23:X23"/>
+    <mergeCell ref="Y23:AC23"/>
+    <mergeCell ref="AD23:AH23"/>
+    <mergeCell ref="T24:X24"/>
+    <mergeCell ref="Y24:AC24"/>
+    <mergeCell ref="AD24:AH24"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AH29"/>
+    <mergeCell ref="T30:X30"/>
+    <mergeCell ref="Y30:AC30"/>
+    <mergeCell ref="AD30:AH30"/>
+    <mergeCell ref="T27:X27"/>
+    <mergeCell ref="Y27:AC27"/>
+    <mergeCell ref="AD27:AH27"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="Y28:AC28"/>
+    <mergeCell ref="AD28:AH28"/>
+    <mergeCell ref="T33:X33"/>
+    <mergeCell ref="Y33:AC33"/>
+    <mergeCell ref="AD33:AH33"/>
+    <mergeCell ref="T36:X36"/>
+    <mergeCell ref="Y36:AC36"/>
+    <mergeCell ref="AD36:AH36"/>
+    <mergeCell ref="T31:X31"/>
+    <mergeCell ref="Y31:AC31"/>
+    <mergeCell ref="AD31:AH31"/>
+    <mergeCell ref="T32:X32"/>
+    <mergeCell ref="Y32:AC32"/>
+    <mergeCell ref="AD32:AH32"/>
+    <mergeCell ref="T34:X34"/>
+    <mergeCell ref="Y34:AC34"/>
+    <mergeCell ref="AD34:AH34"/>
+    <mergeCell ref="T35:X35"/>
+    <mergeCell ref="Y35:AC35"/>
+    <mergeCell ref="AD35:AH35"/>
+    <mergeCell ref="T39:X39"/>
+    <mergeCell ref="Y39:AC39"/>
+    <mergeCell ref="AD39:AH39"/>
+    <mergeCell ref="T40:X40"/>
+    <mergeCell ref="Y40:AC40"/>
+    <mergeCell ref="AD40:AH40"/>
+    <mergeCell ref="T37:X37"/>
+    <mergeCell ref="Y37:AC37"/>
+    <mergeCell ref="AD37:AH37"/>
+    <mergeCell ref="T38:X38"/>
+    <mergeCell ref="Y38:AC38"/>
+    <mergeCell ref="AD38:AH38"/>
+    <mergeCell ref="T41:X41"/>
+    <mergeCell ref="Y41:AC41"/>
+    <mergeCell ref="AD41:AH41"/>
+    <mergeCell ref="T42:X42"/>
+    <mergeCell ref="Y42:AC42"/>
+    <mergeCell ref="AD42:AH42"/>
+    <mergeCell ref="T48:X48"/>
+    <mergeCell ref="Y48:AC48"/>
+    <mergeCell ref="AD48:AH48"/>
+    <mergeCell ref="T44:X44"/>
+    <mergeCell ref="Y51:AC51"/>
+    <mergeCell ref="AD52:AH52"/>
+    <mergeCell ref="AD66:AH66"/>
+    <mergeCell ref="T67:X67"/>
+    <mergeCell ref="Y67:AC67"/>
+    <mergeCell ref="AD67:AH67"/>
+    <mergeCell ref="T64:X64"/>
+    <mergeCell ref="Y64:AC64"/>
+    <mergeCell ref="T43:X43"/>
+    <mergeCell ref="Y43:AC43"/>
+    <mergeCell ref="AD43:AH43"/>
+    <mergeCell ref="T47:X47"/>
+    <mergeCell ref="Y47:AC47"/>
+    <mergeCell ref="AD47:AH47"/>
+    <mergeCell ref="T49:X49"/>
+    <mergeCell ref="Y49:AC49"/>
+    <mergeCell ref="AD49:AH49"/>
+    <mergeCell ref="AD50:AH50"/>
+    <mergeCell ref="AD59:AH59"/>
+    <mergeCell ref="T52:X52"/>
+    <mergeCell ref="Y52:AC52"/>
+    <mergeCell ref="T58:X58"/>
+    <mergeCell ref="Y58:AC58"/>
+    <mergeCell ref="AD58:AH58"/>
+    <mergeCell ref="T59:X59"/>
+    <mergeCell ref="Y59:AC59"/>
+    <mergeCell ref="F71:AD71"/>
+    <mergeCell ref="T66:X66"/>
+    <mergeCell ref="Y66:AC66"/>
+    <mergeCell ref="Y44:AC44"/>
+    <mergeCell ref="AD44:AH44"/>
+    <mergeCell ref="T45:X45"/>
+    <mergeCell ref="Y45:AC45"/>
+    <mergeCell ref="AD45:AH45"/>
+    <mergeCell ref="T46:X46"/>
+    <mergeCell ref="Y46:AC46"/>
+    <mergeCell ref="F70:AD70"/>
+    <mergeCell ref="AD51:AH51"/>
+    <mergeCell ref="T53:X53"/>
+    <mergeCell ref="Y53:AC53"/>
+    <mergeCell ref="AD53:AH53"/>
+    <mergeCell ref="T50:X50"/>
+    <mergeCell ref="Y50:AC50"/>
+    <mergeCell ref="AD46:AH46"/>
+    <mergeCell ref="T51:X51"/>
+    <mergeCell ref="T56:X56"/>
+    <mergeCell ref="Y56:AC56"/>
+    <mergeCell ref="AD56:AH56"/>
+    <mergeCell ref="T57:X57"/>
+    <mergeCell ref="Y57:AC57"/>
+    <mergeCell ref="AD57:AH57"/>
+    <mergeCell ref="T54:X54"/>
+    <mergeCell ref="Y54:AC54"/>
+    <mergeCell ref="AD54:AH54"/>
+    <mergeCell ref="T55:X55"/>
+    <mergeCell ref="Y55:AC55"/>
+    <mergeCell ref="AD55:AH55"/>
     <mergeCell ref="T60:X60"/>
     <mergeCell ref="Y60:AC60"/>
     <mergeCell ref="AD60:AH60"/>
@@ -11912,191 +12321,70 @@
     <mergeCell ref="Y61:AC61"/>
     <mergeCell ref="AD61:AH61"/>
     <mergeCell ref="AE70:AH70"/>
-    <mergeCell ref="T57:X57"/>
-    <mergeCell ref="Y57:AC57"/>
-    <mergeCell ref="AD57:AH57"/>
-    <mergeCell ref="T54:X54"/>
-    <mergeCell ref="Y54:AC54"/>
-    <mergeCell ref="AD54:AH54"/>
-    <mergeCell ref="T55:X55"/>
-    <mergeCell ref="Y55:AC55"/>
-    <mergeCell ref="AD55:AH55"/>
-    <mergeCell ref="T59:X59"/>
-    <mergeCell ref="Y59:AC59"/>
-    <mergeCell ref="F71:AD71"/>
-    <mergeCell ref="T66:X66"/>
-    <mergeCell ref="Y66:AC66"/>
-    <mergeCell ref="Y44:AC44"/>
-    <mergeCell ref="AD44:AH44"/>
-    <mergeCell ref="T45:X45"/>
-    <mergeCell ref="Y45:AC45"/>
-    <mergeCell ref="AD45:AH45"/>
-    <mergeCell ref="T46:X46"/>
-    <mergeCell ref="Y46:AC46"/>
-    <mergeCell ref="F70:AD70"/>
-    <mergeCell ref="AD51:AH51"/>
-    <mergeCell ref="T53:X53"/>
-    <mergeCell ref="Y53:AC53"/>
-    <mergeCell ref="AD53:AH53"/>
-    <mergeCell ref="T50:X50"/>
-    <mergeCell ref="Y50:AC50"/>
-    <mergeCell ref="AD46:AH46"/>
-    <mergeCell ref="T51:X51"/>
-    <mergeCell ref="T56:X56"/>
-    <mergeCell ref="Y56:AC56"/>
-    <mergeCell ref="AD56:AH56"/>
-    <mergeCell ref="Y51:AC51"/>
-    <mergeCell ref="AD52:AH52"/>
-    <mergeCell ref="AD66:AH66"/>
-    <mergeCell ref="T67:X67"/>
-    <mergeCell ref="Y67:AC67"/>
-    <mergeCell ref="AD67:AH67"/>
-    <mergeCell ref="T64:X64"/>
-    <mergeCell ref="Y64:AC64"/>
-    <mergeCell ref="T43:X43"/>
-    <mergeCell ref="Y43:AC43"/>
-    <mergeCell ref="AD43:AH43"/>
-    <mergeCell ref="T47:X47"/>
-    <mergeCell ref="Y47:AC47"/>
-    <mergeCell ref="AD47:AH47"/>
-    <mergeCell ref="T49:X49"/>
-    <mergeCell ref="Y49:AC49"/>
-    <mergeCell ref="AD49:AH49"/>
-    <mergeCell ref="AD50:AH50"/>
-    <mergeCell ref="AD59:AH59"/>
-    <mergeCell ref="T52:X52"/>
-    <mergeCell ref="Y52:AC52"/>
-    <mergeCell ref="T58:X58"/>
-    <mergeCell ref="Y58:AC58"/>
-    <mergeCell ref="AD58:AH58"/>
-    <mergeCell ref="T41:X41"/>
-    <mergeCell ref="Y41:AC41"/>
-    <mergeCell ref="AD41:AH41"/>
-    <mergeCell ref="T42:X42"/>
-    <mergeCell ref="Y42:AC42"/>
-    <mergeCell ref="AD42:AH42"/>
-    <mergeCell ref="T48:X48"/>
-    <mergeCell ref="Y48:AC48"/>
-    <mergeCell ref="AD48:AH48"/>
-    <mergeCell ref="T44:X44"/>
-    <mergeCell ref="T39:X39"/>
-    <mergeCell ref="Y39:AC39"/>
-    <mergeCell ref="AD39:AH39"/>
-    <mergeCell ref="T40:X40"/>
-    <mergeCell ref="Y40:AC40"/>
-    <mergeCell ref="AD40:AH40"/>
-    <mergeCell ref="T37:X37"/>
-    <mergeCell ref="Y37:AC37"/>
-    <mergeCell ref="AD37:AH37"/>
-    <mergeCell ref="T38:X38"/>
-    <mergeCell ref="Y38:AC38"/>
-    <mergeCell ref="AD38:AH38"/>
-    <mergeCell ref="T33:X33"/>
-    <mergeCell ref="Y33:AC33"/>
-    <mergeCell ref="AD33:AH33"/>
-    <mergeCell ref="T36:X36"/>
-    <mergeCell ref="Y36:AC36"/>
-    <mergeCell ref="AD36:AH36"/>
-    <mergeCell ref="T31:X31"/>
-    <mergeCell ref="Y31:AC31"/>
-    <mergeCell ref="AD31:AH31"/>
-    <mergeCell ref="T32:X32"/>
-    <mergeCell ref="Y32:AC32"/>
-    <mergeCell ref="AD32:AH32"/>
-    <mergeCell ref="T34:X34"/>
-    <mergeCell ref="Y34:AC34"/>
-    <mergeCell ref="AD34:AH34"/>
-    <mergeCell ref="T35:X35"/>
-    <mergeCell ref="Y35:AC35"/>
-    <mergeCell ref="AD35:AH35"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AH29"/>
-    <mergeCell ref="T30:X30"/>
-    <mergeCell ref="Y30:AC30"/>
-    <mergeCell ref="AD30:AH30"/>
-    <mergeCell ref="T27:X27"/>
-    <mergeCell ref="Y27:AC27"/>
-    <mergeCell ref="AD27:AH27"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="Y28:AC28"/>
-    <mergeCell ref="AD28:AH28"/>
-    <mergeCell ref="T26:X26"/>
-    <mergeCell ref="Y26:AC26"/>
-    <mergeCell ref="AD26:AH26"/>
-    <mergeCell ref="T23:X23"/>
-    <mergeCell ref="Y23:AC23"/>
-    <mergeCell ref="AD23:AH23"/>
-    <mergeCell ref="T24:X24"/>
-    <mergeCell ref="Y24:AC24"/>
-    <mergeCell ref="AD24:AH24"/>
-    <mergeCell ref="AD22:AH22"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="Y19:AC19"/>
-    <mergeCell ref="AD19:AH19"/>
-    <mergeCell ref="T20:X20"/>
-    <mergeCell ref="Y20:AC20"/>
-    <mergeCell ref="AD20:AH20"/>
-    <mergeCell ref="T25:X25"/>
-    <mergeCell ref="Y25:AC25"/>
-    <mergeCell ref="AD25:AH25"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="Y3:AC3"/>
-    <mergeCell ref="AD3:AH3"/>
-    <mergeCell ref="T12:X12"/>
-    <mergeCell ref="Y12:AC12"/>
-    <mergeCell ref="AD12:AH12"/>
-    <mergeCell ref="T10:X10"/>
-    <mergeCell ref="Y10:AC10"/>
-    <mergeCell ref="AD10:AH10"/>
-    <mergeCell ref="T11:X11"/>
-    <mergeCell ref="Y11:AC11"/>
-    <mergeCell ref="AD11:AH11"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="Y9:AC9"/>
-    <mergeCell ref="AD9:AH9"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="Y5:AC5"/>
-    <mergeCell ref="AD5:AH5"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="Y4:AC4"/>
-    <mergeCell ref="AD4:AH4"/>
-    <mergeCell ref="T6:X6"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AD6:AH6"/>
-    <mergeCell ref="T7:X7"/>
-    <mergeCell ref="Y7:AC7"/>
-    <mergeCell ref="AD7:AH7"/>
-    <mergeCell ref="T8:X8"/>
-    <mergeCell ref="Y8:AC8"/>
-    <mergeCell ref="AD8:AH8"/>
-    <mergeCell ref="T14:X14"/>
-    <mergeCell ref="Y14:AC14"/>
-    <mergeCell ref="AD14:AH14"/>
-    <mergeCell ref="AD15:AH15"/>
-    <mergeCell ref="T16:X16"/>
-    <mergeCell ref="Y16:AC16"/>
-    <mergeCell ref="T13:X13"/>
-    <mergeCell ref="Y13:AC13"/>
-    <mergeCell ref="AD13:AH13"/>
-    <mergeCell ref="N108:AC108"/>
-    <mergeCell ref="AD108:AH108"/>
-    <mergeCell ref="N109:AC109"/>
-    <mergeCell ref="AD109:AH109"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="Y17:AC17"/>
-    <mergeCell ref="AD17:AH17"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="Y18:AC18"/>
-    <mergeCell ref="AD18:AH18"/>
-    <mergeCell ref="T15:X15"/>
-    <mergeCell ref="Y15:AC15"/>
-    <mergeCell ref="AD16:AH16"/>
-    <mergeCell ref="T21:X21"/>
-    <mergeCell ref="Y21:AC21"/>
-    <mergeCell ref="AD21:AH21"/>
-    <mergeCell ref="T22:X22"/>
-    <mergeCell ref="Y22:AC22"/>
+    <mergeCell ref="J77:AH77"/>
+    <mergeCell ref="T68:X68"/>
+    <mergeCell ref="Y68:AC68"/>
+    <mergeCell ref="AD68:AH68"/>
+    <mergeCell ref="K84:R84"/>
+    <mergeCell ref="K85:R85"/>
+    <mergeCell ref="K86:R86"/>
+    <mergeCell ref="J76:AH76"/>
+    <mergeCell ref="AE74:AH74"/>
+    <mergeCell ref="AE75:AH75"/>
+    <mergeCell ref="F72:AD72"/>
+    <mergeCell ref="F73:AD73"/>
+    <mergeCell ref="F74:AD74"/>
+    <mergeCell ref="F75:AD75"/>
+    <mergeCell ref="AE71:AH71"/>
+    <mergeCell ref="AE72:AH72"/>
+    <mergeCell ref="K87:R87"/>
+    <mergeCell ref="S81:Z81"/>
+    <mergeCell ref="S82:Z82"/>
+    <mergeCell ref="S83:Z83"/>
+    <mergeCell ref="S84:Z84"/>
+    <mergeCell ref="S85:Z85"/>
+    <mergeCell ref="S90:Z90"/>
+    <mergeCell ref="AA90:AH90"/>
+    <mergeCell ref="S87:Z87"/>
+    <mergeCell ref="AA81:AH81"/>
+    <mergeCell ref="AA82:AH82"/>
+    <mergeCell ref="AA83:AH83"/>
+    <mergeCell ref="AA84:AH84"/>
+    <mergeCell ref="AA85:AH85"/>
+    <mergeCell ref="AA86:AH86"/>
+    <mergeCell ref="AA87:AH87"/>
+    <mergeCell ref="S86:Z86"/>
+    <mergeCell ref="AA91:AH91"/>
+    <mergeCell ref="AA92:AH92"/>
+    <mergeCell ref="AA93:AH93"/>
+    <mergeCell ref="AA94:AH94"/>
+    <mergeCell ref="AA95:AH95"/>
+    <mergeCell ref="AA96:AH96"/>
+    <mergeCell ref="AA97:AH97"/>
+    <mergeCell ref="AA98:AH98"/>
+    <mergeCell ref="S97:Z97"/>
+    <mergeCell ref="S98:Z98"/>
+    <mergeCell ref="S91:Z91"/>
+    <mergeCell ref="S92:Z92"/>
+    <mergeCell ref="S93:Z93"/>
+    <mergeCell ref="S94:Z94"/>
+    <mergeCell ref="S95:Z95"/>
+    <mergeCell ref="S96:Z96"/>
+    <mergeCell ref="C107:M107"/>
+    <mergeCell ref="N107:AC107"/>
+    <mergeCell ref="AD107:AH107"/>
+    <mergeCell ref="AA99:AH99"/>
+    <mergeCell ref="AA100:AH100"/>
+    <mergeCell ref="AA101:AH101"/>
+    <mergeCell ref="AA102:AH102"/>
+    <mergeCell ref="AA103:AH103"/>
+    <mergeCell ref="AA104:AH104"/>
+    <mergeCell ref="S103:Z103"/>
+    <mergeCell ref="S104:Z104"/>
+    <mergeCell ref="S99:Z99"/>
+    <mergeCell ref="S100:Z100"/>
+    <mergeCell ref="S101:Z101"/>
+    <mergeCell ref="S102:Z102"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AI52" r:id="rId1" display="JMP@R3" xr:uid="{00000000-0004-0000-0300-000000000000}"/>

</xml_diff>